<commit_message>
spreadsheet updates as per ml cheatsheet
</commit_message>
<xml_diff>
--- a/docs/Book1.xlsx
+++ b/docs/Book1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="570" yWindow="450" windowWidth="18585" windowHeight="10740"/>
+    <workbookView xWindow="4290" yWindow="495" windowWidth="18585" windowHeight="10740"/>
   </bookViews>
   <sheets>
     <sheet name="activation test data (2)" sheetId="2" r:id="rId1"/>
@@ -12,12 +12,26 @@
     <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
+    <definedName name="A">'activation test data (2)'!$C$43:$E$44</definedName>
+    <definedName name="ActivationH">'activation test data (2)'!$K$9:$K$12</definedName>
+    <definedName name="ActivationHidden">'activation test data (2)'!$Q$9:$Q$18</definedName>
+    <definedName name="ActivationO">'activation test data (2)'!$O$26:$O$35</definedName>
+    <definedName name="AX">'activation test data (2)'!$C$49:$C$50</definedName>
+    <definedName name="BiasDerivativeH">'activation test data (2)'!$L$9:$L$12</definedName>
+    <definedName name="BiasDerivativeO">'activation test data (2)'!$P$26:$P$35</definedName>
     <definedName name="BiasH">'activation test data (2)'!$E$20:$H$20</definedName>
-    <definedName name="BiasOutput">'activation test data (2)'!$C$38:$L$38</definedName>
+    <definedName name="BiasO">'activation test data (2)'!$C$32:$L$32</definedName>
+    <definedName name="Eh">'activation test data (2)'!$G$39:$G$48</definedName>
+    <definedName name="Eo">'activation test data (2)'!$E$39:$E$48</definedName>
     <definedName name="InputX">'activation test data (2)'!$B$9:$B$18</definedName>
+    <definedName name="label">'activation test data (2)'!$C$9:$C$18</definedName>
     <definedName name="WeightsH">'activation test data (2)'!$E$9:$H$18</definedName>
-    <definedName name="WeightsOuput">'activation test data (2)'!$C$26:$L$35</definedName>
-    <definedName name="Z">'activation test data (2)'!$J$9:$J$18</definedName>
+    <definedName name="WeightsO">'activation test data (2)'!$C$26:$L$29</definedName>
+    <definedName name="X">'activation test data (2)'!$C$46:$E$46</definedName>
+    <definedName name="XX">'activation test data (2)'!$G$43:$G$45</definedName>
+    <definedName name="Zh">'activation test data (2)'!$J$9:$J$12</definedName>
+    <definedName name="ZhWRONG">'activation test data (2)'!$P$9:$P$12</definedName>
+    <definedName name="Zo">'activation test data (2)'!$N$26:$N$35</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
   <extLst>
@@ -34,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
   <si>
     <t>input</t>
   </si>
@@ -69,18 +83,9 @@
     <t>WeightsH</t>
   </si>
   <si>
-    <t>Z</t>
-  </si>
-  <si>
     <t>BiasH</t>
   </si>
   <si>
-    <t>Activation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bias </t>
-  </si>
-  <si>
     <t>Derivative</t>
   </si>
   <si>
@@ -96,30 +101,61 @@
     <t>Weight</t>
   </si>
   <si>
-    <t>Hidden Layer</t>
-  </si>
-  <si>
-    <t>Output</t>
-  </si>
-  <si>
     <t>&lt;- neurons -&gt;</t>
   </si>
   <si>
     <t>OUTPUT LAYER</t>
   </si>
   <si>
-    <t>WeightsOutput</t>
-  </si>
-  <si>
     <t>BiasOutput</t>
+  </si>
+  <si>
+    <t>Zh</t>
+  </si>
+  <si>
+    <t>BiasDerivativeH</t>
+  </si>
+  <si>
+    <t>ActivationH</t>
+  </si>
+  <si>
+    <t>Zo</t>
+  </si>
+  <si>
+    <t>ActivationO</t>
+  </si>
+  <si>
+    <t>BiasDerivativeO</t>
+  </si>
+  <si>
+    <t>WeightsO</t>
+  </si>
+  <si>
+    <t>Input Layer</t>
+  </si>
+  <si>
+    <t>Eo</t>
+  </si>
+  <si>
+    <t>Prime Zo</t>
+  </si>
+  <si>
+    <t>Eh</t>
+  </si>
+  <si>
+    <t>dWo = Eo * H</t>
+  </si>
+  <si>
+    <t>H</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.0000000"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -213,7 +249,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
@@ -221,6 +257,7 @@
     <xf numFmtId="164" fontId="2" fillId="3" borderId="1" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Calculation" xfId="3" builtinId="22"/>
@@ -530,7 +567,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -538,10 +575,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B5:Q38"/>
+  <dimension ref="B4:U48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="L36" sqref="L36"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -557,7 +594,8 @@
     <col min="11" max="11" width="15.5703125" customWidth="1"/>
     <col min="12" max="12" width="13.85546875" customWidth="1"/>
     <col min="13" max="13" width="11.85546875" customWidth="1"/>
-    <col min="15" max="15" width="11" customWidth="1"/>
+    <col min="14" max="14" width="12" customWidth="1"/>
+    <col min="15" max="15" width="13.5703125" customWidth="1"/>
     <col min="16" max="16" width="10.140625" customWidth="1"/>
     <col min="18" max="18" width="12" customWidth="1"/>
     <col min="19" max="19" width="11" customWidth="1"/>
@@ -572,69 +610,65 @@
     <col min="31" max="31" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="K5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="F6" t="s">
+    <row r="4" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="O4" s="7"/>
+    </row>
+    <row r="5" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="K5" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="F6" s="6" t="s">
         <v>9</v>
       </c>
       <c r="K6" t="s">
+        <v>15</v>
+      </c>
+      <c r="L6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B7" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" t="s">
         <v>17</v>
       </c>
-      <c r="L6" t="s">
+      <c r="K7" t="s">
+        <v>14</v>
+      </c>
+      <c r="T7" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>0</v>
-      </c>
-      <c r="F7" t="s">
-        <v>22</v>
-      </c>
-      <c r="K7" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="L7" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="N7" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q7" s="6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
+      <c r="U7" s="6"/>
+    </row>
+    <row r="8" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B8" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="6" t="s">
         <v>8</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>10</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="K8" s="6" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="L8" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="N8" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q8" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="T8" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="U8" s="6"/>
+    </row>
+    <row r="9" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B9" s="4">
         <v>1</v>
       </c>
@@ -654,7 +688,7 @@
         <v>1</v>
       </c>
       <c r="J9" s="5">
-        <f t="array" ref="J9:J18">WeightsH* TRANSPOSE( InputX)+BiasH</f>
+        <f t="array" ref="J9:J12">MMULT(TRANSPOSE(WeightsH),InputX)+TRANSPOSE(BiasH)</f>
         <v>1.5</v>
       </c>
       <c r="K9" s="5">
@@ -665,11 +699,8 @@
         <f>1/(1+EXP(-J9))*(1-(1/(1+EXP(-J9))))</f>
         <v>0.14914645207033286</v>
       </c>
-      <c r="Q9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="2:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B10" s="4">
         <v>0</v>
       </c>
@@ -692,18 +723,15 @@
         <v>1.5</v>
       </c>
       <c r="K10" s="5">
-        <f t="shared" ref="K10:K18" si="0">1/(1+EXP(-J10))</f>
+        <f t="shared" ref="K10:K12" si="0">1/(1+EXP(-J10))</f>
         <v>0.81757447619364365</v>
       </c>
       <c r="L10" s="5">
-        <f t="shared" ref="L10:L18" si="1">1/(1+EXP(-J10))*(1-(1/(1+EXP(-J10))))</f>
+        <f t="shared" ref="L10:L12" si="1">1/(1+EXP(-J10))*(1-(1/(1+EXP(-J10))))</f>
         <v>0.14914645207033286</v>
       </c>
-      <c r="Q10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="2:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B11" s="4">
         <v>0</v>
       </c>
@@ -733,11 +761,8 @@
         <f t="shared" si="1"/>
         <v>0.14914645207033286</v>
       </c>
-      <c r="Q11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="2:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B12" s="4">
         <v>0</v>
       </c>
@@ -767,11 +792,8 @@
         <f t="shared" si="1"/>
         <v>0.14914645207033286</v>
       </c>
-      <c r="Q12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B13" s="4">
         <v>0</v>
       </c>
@@ -790,22 +812,8 @@
       <c r="H13" s="2">
         <v>1</v>
       </c>
-      <c r="J13" s="5">
-        <v>1.5</v>
-      </c>
-      <c r="K13" s="5">
-        <f t="shared" si="0"/>
-        <v>0.81757447619364365</v>
-      </c>
-      <c r="L13" s="5">
-        <f t="shared" si="1"/>
-        <v>0.14914645207033286</v>
-      </c>
-      <c r="Q13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B14" s="4">
         <v>0</v>
       </c>
@@ -824,22 +832,8 @@
       <c r="H14" s="2">
         <v>1</v>
       </c>
-      <c r="J14" s="5">
-        <v>1.5</v>
-      </c>
-      <c r="K14" s="5">
-        <f t="shared" si="0"/>
-        <v>0.81757447619364365</v>
-      </c>
-      <c r="L14" s="5">
-        <f t="shared" si="1"/>
-        <v>0.14914645207033286</v>
-      </c>
-      <c r="Q14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="2:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B15" s="4">
         <v>0</v>
       </c>
@@ -858,22 +852,8 @@
       <c r="H15" s="2">
         <v>1</v>
       </c>
-      <c r="J15" s="5">
-        <v>1.5</v>
-      </c>
-      <c r="K15" s="5">
-        <f t="shared" si="0"/>
-        <v>0.81757447619364365</v>
-      </c>
-      <c r="L15" s="5">
-        <f t="shared" si="1"/>
-        <v>0.14914645207033286</v>
-      </c>
-      <c r="Q15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="2:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B16" s="4">
         <v>0</v>
       </c>
@@ -892,22 +872,8 @@
       <c r="H16" s="2">
         <v>1</v>
       </c>
-      <c r="J16" s="5">
-        <v>1.5</v>
-      </c>
-      <c r="K16" s="5">
-        <f t="shared" si="0"/>
-        <v>0.81757447619364365</v>
-      </c>
-      <c r="L16" s="5">
-        <f t="shared" si="1"/>
-        <v>0.14914645207033286</v>
-      </c>
-      <c r="Q16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="2:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B17" s="4">
         <v>0</v>
       </c>
@@ -926,22 +892,8 @@
       <c r="H17" s="2">
         <v>1</v>
       </c>
-      <c r="J17" s="5">
-        <v>1.5</v>
-      </c>
-      <c r="K17" s="5">
-        <f t="shared" si="0"/>
-        <v>0.81757447619364365</v>
-      </c>
-      <c r="L17" s="5">
-        <f t="shared" si="1"/>
-        <v>0.14914645207033286</v>
-      </c>
-      <c r="Q17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="2:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B18" s="4">
         <v>0</v>
       </c>
@@ -960,24 +912,10 @@
       <c r="H18" s="2">
         <v>1</v>
       </c>
-      <c r="J18" s="5">
-        <v>1.5</v>
-      </c>
-      <c r="K18" s="5">
-        <f t="shared" si="0"/>
-        <v>0.81757447619364365</v>
-      </c>
-      <c r="L18" s="5">
-        <f t="shared" si="1"/>
-        <v>0.14914645207033286</v>
-      </c>
-      <c r="Q18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="D20" t="s">
-        <v>12</v>
+    </row>
+    <row r="20" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="D20" s="6" t="s">
+        <v>11</v>
       </c>
       <c r="E20" s="2">
         <v>0.5</v>
@@ -992,22 +930,34 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="23" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="D23" t="s">
+    <row r="23" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="D23" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="D24" t="s">
+        <v>17</v>
+      </c>
+      <c r="P24" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C25" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="N25" s="6" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="24" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="D24" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="25" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="C25" s="3" t="s">
+      <c r="O25" s="6" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="P25" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C26" s="2">
         <v>1</v>
       </c>
@@ -1038,8 +988,20 @@
       <c r="L26" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="N26" s="5">
+        <f t="array" ref="N26:N35">MMULT(TRANSPOSE(WeightsO), ActivationH) +TRANSPOSE(BiasO)</f>
+        <v>3.7702979047745746</v>
+      </c>
+      <c r="O26" s="5">
+        <f>1/(1+EXP(-N26))</f>
+        <v>0.97747392093906782</v>
+      </c>
+      <c r="P26" s="5">
+        <f>1/(1+EXP(-N26))*(1-(1/(1+EXP(-N26))))</f>
+        <v>2.2018654823072813E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C27" s="2">
         <v>1</v>
       </c>
@@ -1070,8 +1032,19 @@
       <c r="L27" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="N27" s="5">
+        <v>3.7702979047745746</v>
+      </c>
+      <c r="O27" s="5">
+        <f t="shared" ref="O27:O35" si="2">1/(1+EXP(-N27))</f>
+        <v>0.97747392093906782</v>
+      </c>
+      <c r="P27" s="5">
+        <f t="shared" ref="P27:P35" si="3">1/(1+EXP(-N27))*(1-(1/(1+EXP(-N27))))</f>
+        <v>2.2018654823072813E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C28" s="2">
         <v>1</v>
       </c>
@@ -1102,8 +1075,19 @@
       <c r="L28" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="N28" s="5">
+        <v>3.7702979047745746</v>
+      </c>
+      <c r="O28" s="5">
+        <f t="shared" si="2"/>
+        <v>0.97747392093906782</v>
+      </c>
+      <c r="P28" s="5">
+        <f t="shared" si="3"/>
+        <v>2.2018654823072813E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C29" s="2">
         <v>1</v>
       </c>
@@ -1134,234 +1118,220 @@
       <c r="L29" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="C30" s="2">
-        <v>1</v>
-      </c>
-      <c r="D30" s="2">
-        <v>1</v>
-      </c>
-      <c r="E30" s="2">
-        <v>1</v>
-      </c>
-      <c r="F30" s="2">
-        <v>1</v>
-      </c>
-      <c r="G30" s="2">
-        <v>1</v>
-      </c>
-      <c r="H30" s="2">
-        <v>1</v>
-      </c>
-      <c r="I30" s="2">
-        <v>1</v>
-      </c>
-      <c r="J30" s="2">
-        <v>1</v>
-      </c>
-      <c r="K30" s="2">
-        <v>1</v>
-      </c>
-      <c r="L30" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="C31" s="2">
-        <v>1</v>
-      </c>
-      <c r="D31" s="2">
-        <v>1</v>
-      </c>
-      <c r="E31" s="2">
-        <v>1</v>
-      </c>
-      <c r="F31" s="2">
-        <v>1</v>
-      </c>
-      <c r="G31" s="2">
-        <v>1</v>
-      </c>
-      <c r="H31" s="2">
-        <v>1</v>
-      </c>
-      <c r="I31" s="2">
-        <v>1</v>
-      </c>
-      <c r="J31" s="2">
-        <v>1</v>
-      </c>
-      <c r="K31" s="2">
-        <v>1</v>
-      </c>
-      <c r="L31" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="N29" s="5">
+        <v>3.7702979047745746</v>
+      </c>
+      <c r="O29" s="5">
+        <f t="shared" si="2"/>
+        <v>0.97747392093906782</v>
+      </c>
+      <c r="P29" s="5">
+        <f t="shared" si="3"/>
+        <v>2.2018654823072813E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="N30" s="5">
+        <v>3.7702979047745746</v>
+      </c>
+      <c r="O30" s="5">
+        <f t="shared" si="2"/>
+        <v>0.97747392093906782</v>
+      </c>
+      <c r="P30" s="5">
+        <f t="shared" si="3"/>
+        <v>2.2018654823072813E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C31" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="N31" s="5">
+        <v>3.7702979047745746</v>
+      </c>
+      <c r="O31" s="5">
+        <f t="shared" si="2"/>
+        <v>0.97747392093906782</v>
+      </c>
+      <c r="P31" s="5">
+        <f t="shared" si="3"/>
+        <v>2.2018654823072813E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C32" s="2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="D32" s="2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="E32" s="2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="F32" s="2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="G32" s="2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="H32" s="2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="I32" s="2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J32" s="2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="K32" s="2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="L32" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C33" s="2">
-        <v>1</v>
-      </c>
-      <c r="D33" s="2">
-        <v>1</v>
-      </c>
-      <c r="E33" s="2">
-        <v>1</v>
-      </c>
-      <c r="F33" s="2">
-        <v>1</v>
-      </c>
-      <c r="G33" s="2">
-        <v>1</v>
-      </c>
-      <c r="H33" s="2">
-        <v>1</v>
-      </c>
-      <c r="I33" s="2">
-        <v>1</v>
-      </c>
-      <c r="J33" s="2">
-        <v>1</v>
-      </c>
-      <c r="K33" s="2">
-        <v>1</v>
-      </c>
-      <c r="L33" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C34" s="2">
-        <v>1</v>
-      </c>
-      <c r="D34" s="2">
-        <v>1</v>
-      </c>
-      <c r="E34" s="2">
-        <v>1</v>
-      </c>
-      <c r="F34" s="2">
-        <v>1</v>
-      </c>
-      <c r="G34" s="2">
-        <v>1</v>
-      </c>
-      <c r="H34" s="2">
-        <v>1</v>
-      </c>
-      <c r="I34" s="2">
-        <v>1</v>
-      </c>
-      <c r="J34" s="2">
-        <v>1</v>
-      </c>
-      <c r="K34" s="2">
-        <v>1</v>
-      </c>
-      <c r="L34" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C35" s="2">
-        <v>1</v>
-      </c>
-      <c r="D35" s="2">
-        <v>1</v>
-      </c>
-      <c r="E35" s="2">
-        <v>1</v>
-      </c>
-      <c r="F35" s="2">
-        <v>1</v>
-      </c>
-      <c r="G35" s="2">
-        <v>1</v>
-      </c>
-      <c r="H35" s="2">
-        <v>1</v>
-      </c>
-      <c r="I35" s="2">
-        <v>1</v>
-      </c>
-      <c r="J35" s="2">
-        <v>1</v>
-      </c>
-      <c r="K35" s="2">
-        <v>1</v>
-      </c>
-      <c r="L35" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C37" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="38" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C38" s="2">
         <v>0.5</v>
       </c>
-      <c r="D38" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="E38" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="F38" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="G38" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="H38" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="I38" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="J38" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="K38" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="L38" s="2">
-        <v>0.5</v>
+      <c r="N32" s="5">
+        <v>3.7702979047745746</v>
+      </c>
+      <c r="O32" s="5">
+        <f t="shared" si="2"/>
+        <v>0.97747392093906782</v>
+      </c>
+      <c r="P32" s="5">
+        <f t="shared" si="3"/>
+        <v>2.2018654823072813E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="N33" s="5">
+        <v>3.7702979047745746</v>
+      </c>
+      <c r="O33" s="5">
+        <f t="shared" si="2"/>
+        <v>0.97747392093906782</v>
+      </c>
+      <c r="P33" s="5">
+        <f t="shared" si="3"/>
+        <v>2.2018654823072813E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="N34" s="5">
+        <v>3.7702979047745746</v>
+      </c>
+      <c r="O34" s="5">
+        <f t="shared" si="2"/>
+        <v>0.97747392093906782</v>
+      </c>
+      <c r="P34" s="5">
+        <f t="shared" si="3"/>
+        <v>2.2018654823072813E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="N35" s="5">
+        <v>3.7702979047745746</v>
+      </c>
+      <c r="O35" s="5">
+        <f t="shared" si="2"/>
+        <v>0.97747392093906782</v>
+      </c>
+      <c r="P35" s="5">
+        <f t="shared" si="3"/>
+        <v>2.2018654823072813E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E38" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="G38" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="I38" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="39" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E39" s="5">
+        <f t="array" ref="E39:E48">(ActivationO-label)*BiasDerivativeO</f>
+        <v>-4.959939593599139E-4</v>
+      </c>
+      <c r="G39" s="5">
+        <f t="array" ref="G39:G48">MMULT(MMULT(Eo,TRANSPOSE(ActivationO)),BiasDerivativeO)</f>
+        <v>-1.0675109777753624E-4</v>
+      </c>
+    </row>
+    <row r="40" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E40" s="5">
+        <v>2.1522660863712899E-2</v>
+      </c>
+      <c r="G40" s="5">
+        <v>4.6322493065439887E-3</v>
+      </c>
+    </row>
+    <row r="41" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E41" s="5">
+        <v>2.1522660863712899E-2</v>
+      </c>
+      <c r="G41" s="5">
+        <v>4.6322493065439887E-3</v>
+      </c>
+    </row>
+    <row r="42" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E42" s="5">
+        <v>2.1522660863712899E-2</v>
+      </c>
+      <c r="G42" s="5">
+        <v>4.6322493065439887E-3</v>
+      </c>
+    </row>
+    <row r="43" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E43" s="5">
+        <v>2.1522660863712899E-2</v>
+      </c>
+      <c r="G43" s="5">
+        <v>4.6322493065439887E-3</v>
+      </c>
+    </row>
+    <row r="44" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E44" s="5">
+        <v>2.1522660863712899E-2</v>
+      </c>
+      <c r="G44" s="5">
+        <v>4.6322493065439887E-3</v>
+      </c>
+    </row>
+    <row r="45" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E45" s="5">
+        <v>2.1522660863712899E-2</v>
+      </c>
+      <c r="G45" s="5">
+        <v>4.6322493065439887E-3</v>
+      </c>
+    </row>
+    <row r="46" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E46" s="5">
+        <v>2.1522660863712899E-2</v>
+      </c>
+      <c r="G46" s="5">
+        <v>4.6322493065439887E-3</v>
+      </c>
+    </row>
+    <row r="47" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E47" s="5">
+        <v>2.1522660863712899E-2</v>
+      </c>
+      <c r="G47" s="5">
+        <v>4.6322493065439887E-3</v>
+      </c>
+    </row>
+    <row r="48" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E48" s="5">
+        <v>2.1522660863712899E-2</v>
+      </c>
+      <c r="G48" s="5">
+        <v>4.6322493065439887E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
reworking for haradman matrix multiplication
</commit_message>
<xml_diff>
--- a/docs/Book1.xlsx
+++ b/docs/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\georgereimer\Source\Repos\neuralNetwork\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21F9896C-4956-4D43-824D-F8E1D574FC56}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD658A82-8622-4155-A5D9-2A70426DDEBC}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4290" yWindow="495" windowWidth="18585" windowHeight="10740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,14 +20,14 @@
   <definedNames>
     <definedName name="A">'activation test data (2)'!$F$54:$H$55</definedName>
     <definedName name="ActivationHidden">'activation test data (2)'!$T$24:$T$24</definedName>
-    <definedName name="AX">'activation test data (2)'!$F$66:$F$67</definedName>
+    <definedName name="AX">'activation test data (2)'!#REF!</definedName>
     <definedName name="BiasDerivativeH">'activation test data (2)'!$R$19:$R$22</definedName>
     <definedName name="BiasDerivativeO">'activation test data (2)'!$R$46:$R$55</definedName>
     <definedName name="BiasH">'activation test data (2)'!$K$25:$N$25</definedName>
     <definedName name="BiasO">'activation test data (2)'!$F$36:$O$36</definedName>
-    <definedName name="dWh">'activation test data (2)'!$F$61:$O$61</definedName>
-    <definedName name="dWo">'activation test data (2)'!$F$61:$I$61+'activation test data (2)'!$F$58:$I$58</definedName>
-    <definedName name="Eh">'activation test data (2)'!$F$55:$O$55</definedName>
+    <definedName name="dWh">'activation test data (2)'!$F$67:$O$67</definedName>
+    <definedName name="dWo">'activation test data (2)'!$F$67:$I$67+'activation test data (2)'!$F$61:$I$61</definedName>
+    <definedName name="Eh">'activation test data (2)'!$F$55:$O$58</definedName>
     <definedName name="Eo">'activation test data (2)'!$F$49:$O$49</definedName>
     <definedName name="H">'activation test data (2)'!$R$13:$U$13</definedName>
     <definedName name="InputX">'activation test data (2)'!#REF!</definedName>
@@ -161,9 +161,6 @@
     <t>4 x 10</t>
   </si>
   <si>
-    <t>X * Wh + BiasH =&gt;</t>
-  </si>
-  <si>
     <t>sigmoid(Zh) =&gt;</t>
   </si>
   <si>
@@ -176,9 +173,6 @@
     <t>OUTPUT LAYER (10)</t>
   </si>
   <si>
-    <t>H * Wo + BiasO =&gt;</t>
-  </si>
-  <si>
     <t>1x4</t>
   </si>
   <si>
@@ -228,6 +222,12 @@
   </si>
   <si>
     <t>meaning</t>
+  </si>
+  <si>
+    <t>dot(X , Wh )+ BiasH =&gt;</t>
+  </si>
+  <si>
+    <t>dot(H , Wo )+ BiasO =&gt;</t>
   </si>
 </sst>
 </file>
@@ -678,10 +678,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:U63"/>
+  <dimension ref="B2:V67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -763,7 +763,7 @@
     </row>
     <row r="6" spans="2:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C6" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E6" s="5"/>
     </row>
@@ -804,7 +804,7 @@
     </row>
     <row r="8" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -839,10 +839,10 @@
     </row>
     <row r="9" spans="2:21" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B9" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="2:21" x14ac:dyDescent="0.25">
@@ -855,13 +855,13 @@
         <v>31</v>
       </c>
       <c r="K11" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="R11" t="s">
         <v>11</v>
       </c>
       <c r="T11" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="2:21" x14ac:dyDescent="0.25">
@@ -894,6 +894,9 @@
       <c r="H13" s="2">
         <v>1</v>
       </c>
+      <c r="I13" s="8" t="s">
+        <v>54</v>
+      </c>
       <c r="K13" s="3">
         <f t="array" ref="K13:N13">MMULT(X,Wh)+BiasH</f>
         <v>0.5</v>
@@ -908,7 +911,7 @@
         <v>0.5</v>
       </c>
       <c r="P13" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="R13" s="3">
         <f>1/(1+EXP(-K13))</f>
@@ -968,9 +971,6 @@
       <c r="H16" s="2">
         <v>1</v>
       </c>
-      <c r="I16" s="8" t="s">
-        <v>33</v>
-      </c>
       <c r="R16" t="s">
         <v>10</v>
       </c>
@@ -1099,7 +1099,7 @@
     </row>
     <row r="27" spans="5:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G27" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="29" spans="5:18" x14ac:dyDescent="0.25">
@@ -1221,7 +1221,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="4:18" x14ac:dyDescent="0.25">
+    <row r="33" spans="4:22" x14ac:dyDescent="0.25">
       <c r="E33" t="s">
         <v>25</v>
       </c>
@@ -1256,12 +1256,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="4:18" x14ac:dyDescent="0.25">
+    <row r="34" spans="4:22" x14ac:dyDescent="0.25">
       <c r="E34" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="35" spans="4:18" x14ac:dyDescent="0.25">
+    <row r="35" spans="4:22" x14ac:dyDescent="0.25">
       <c r="F35" s="4" t="s">
         <v>29</v>
       </c>
@@ -1269,7 +1269,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="36" spans="4:18" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:22" x14ac:dyDescent="0.25">
       <c r="F36" s="2">
         <v>0.5</v>
       </c>
@@ -1301,7 +1301,21 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="38" spans="4:18" x14ac:dyDescent="0.25">
+    <row r="37" spans="4:22" x14ac:dyDescent="0.25">
+      <c r="S37">
+        <v>3</v>
+      </c>
+      <c r="T37">
+        <v>4</v>
+      </c>
+      <c r="U37">
+        <v>2</v>
+      </c>
+      <c r="V37">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="4:22" x14ac:dyDescent="0.25">
       <c r="F38" s="4" t="s">
         <v>15</v>
       </c>
@@ -1309,9 +1323,9 @@
         <v>30</v>
       </c>
     </row>
-    <row r="39" spans="4:18" x14ac:dyDescent="0.25">
+    <row r="39" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D39" s="8" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="F39" s="3">
         <f t="array" ref="F39:O39">MMULT(H,Wo)+BiasO</f>
@@ -1345,14 +1359,26 @@
         <v>2.9898373248074184</v>
       </c>
     </row>
-    <row r="41" spans="4:18" x14ac:dyDescent="0.25">
+    <row r="41" spans="4:22" x14ac:dyDescent="0.25">
       <c r="F41" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="42" spans="4:18" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+      <c r="S41">
+        <v>13</v>
+      </c>
+      <c r="T41">
+        <v>9</v>
+      </c>
+      <c r="U41">
+        <v>7</v>
+      </c>
+      <c r="V41">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="42" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D42" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F42" s="3">
         <f>1/(1+EXP(-F39))</f>
@@ -1394,69 +1420,108 @@
         <f t="shared" si="0"/>
         <v>0.95211289369399577</v>
       </c>
-    </row>
-    <row r="44" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="S42">
+        <v>8</v>
+      </c>
+      <c r="T42">
+        <v>7</v>
+      </c>
+      <c r="U42">
+        <v>4</v>
+      </c>
+      <c r="V42">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="43" spans="4:22" x14ac:dyDescent="0.25">
+      <c r="S43">
+        <v>6</v>
+      </c>
+      <c r="T43">
+        <v>4</v>
+      </c>
+      <c r="U43">
+        <v>0</v>
+      </c>
+      <c r="V43">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="4:22" x14ac:dyDescent="0.25">
       <c r="R44" s="4"/>
     </row>
-    <row r="45" spans="4:18" x14ac:dyDescent="0.25">
+    <row r="45" spans="4:22" x14ac:dyDescent="0.25">
       <c r="F45" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="R45" s="4"/>
     </row>
-    <row r="46" spans="4:18" x14ac:dyDescent="0.25">
+    <row r="46" spans="4:22" x14ac:dyDescent="0.25">
       <c r="F46" s="3">
-        <f>1/(1+EXP(-F39))*(1-(1/(1+EXP(-F39))))</f>
+        <f t="shared" ref="F46:O46" si="1">1/(1+EXP(-F39))*(1-(1/(1+EXP(-F39))))</f>
         <v>4.5593931355641687E-2</v>
       </c>
       <c r="G46" s="3">
-        <f>1/(1+EXP(-G39))*(1-(1/(1+EXP(-G39))))</f>
+        <f t="shared" si="1"/>
         <v>4.5593931355641687E-2</v>
       </c>
       <c r="H46" s="3">
-        <f>1/(1+EXP(-H39))*(1-(1/(1+EXP(-H39))))</f>
+        <f t="shared" si="1"/>
         <v>4.5593931355641687E-2</v>
       </c>
       <c r="I46" s="3">
-        <f>1/(1+EXP(-I39))*(1-(1/(1+EXP(-I39))))</f>
+        <f t="shared" si="1"/>
         <v>4.5593931355641687E-2</v>
       </c>
       <c r="J46" s="3">
-        <f>1/(1+EXP(-J39))*(1-(1/(1+EXP(-J39))))</f>
+        <f t="shared" si="1"/>
         <v>4.5593931355641687E-2</v>
       </c>
       <c r="K46" s="3">
-        <f>1/(1+EXP(-K39))*(1-(1/(1+EXP(-K39))))</f>
+        <f t="shared" si="1"/>
         <v>4.5593931355641687E-2</v>
       </c>
       <c r="L46" s="3">
-        <f>1/(1+EXP(-L39))*(1-(1/(1+EXP(-L39))))</f>
+        <f t="shared" si="1"/>
         <v>4.5593931355641687E-2</v>
       </c>
       <c r="M46" s="3">
-        <f>1/(1+EXP(-M39))*(1-(1/(1+EXP(-M39))))</f>
+        <f t="shared" si="1"/>
         <v>4.5593931355641687E-2</v>
       </c>
       <c r="N46" s="3">
-        <f>1/(1+EXP(-N39))*(1-(1/(1+EXP(-N39))))</f>
+        <f t="shared" si="1"/>
         <v>4.5593931355641687E-2</v>
       </c>
       <c r="O46" s="3">
-        <f>1/(1+EXP(-O39))*(1-(1/(1+EXP(-O39))))</f>
+        <f t="shared" si="1"/>
         <v>4.5593931355641687E-2</v>
       </c>
-    </row>
-    <row r="48" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="S46">
+        <f t="array" ref="S46:V46">MMULT(S37:U37,S41:V43)</f>
+        <v>83</v>
+      </c>
+      <c r="T46">
+        <v>63</v>
+      </c>
+      <c r="U46">
+        <v>37</v>
+      </c>
+      <c r="V46">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="48" spans="4:22" x14ac:dyDescent="0.25">
       <c r="F48" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H48" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="49" spans="2:15" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="49" spans="2:22" x14ac:dyDescent="0.25">
       <c r="D49" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F49" s="3">
         <f t="array" ref="F49:O49">(Output-y)*ZoSigmoidPrime</f>
@@ -1489,143 +1554,383 @@
       <c r="O49" s="3">
         <v>4.3410569917905414E-2</v>
       </c>
-    </row>
-    <row r="51" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="T49">
+        <v>2</v>
+      </c>
+      <c r="U49">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="T50">
+        <v>2</v>
+      </c>
+      <c r="U50">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51" spans="2:22" x14ac:dyDescent="0.25">
       <c r="F51" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="52" spans="2:15" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="52" spans="2:22" x14ac:dyDescent="0.25">
       <c r="F52" s="3">
         <f>1/(1+EXP(-K13))*(1-(1/(1+EXP(-K13))))</f>
         <v>0.23500371220159449</v>
       </c>
       <c r="G52" s="3">
-        <f t="shared" ref="G52:I52" si="1">1/(1+EXP(-L13))*(1-(1/(1+EXP(-L13))))</f>
+        <f t="shared" ref="G52:I52" si="2">1/(1+EXP(-L13))*(1-(1/(1+EXP(-L13))))</f>
         <v>0.23500371220159449</v>
       </c>
       <c r="H52" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.23500371220159449</v>
       </c>
       <c r="I52" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.23500371220159449</v>
       </c>
-    </row>
-    <row r="54" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="T52">
+        <v>3</v>
+      </c>
+      <c r="U52">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="53" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="T53">
+        <v>5</v>
+      </c>
+      <c r="U53">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="54" spans="2:22" x14ac:dyDescent="0.25">
       <c r="F54" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="55" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:22" x14ac:dyDescent="0.25">
       <c r="D55" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F55" s="3">
-        <f t="array" ref="F55:O55">Eo*Wo</f>
-        <v>-2.1833614377362734E-3</v>
+        <f t="array" ref="F55:O58">(Eo*Wo)*ZhSigmoidPrime</f>
+        <v>-5.1309804294583474E-4</v>
       </c>
       <c r="G55" s="3">
-        <v>4.3410569917905414E-2</v>
+        <v>1.0201645079494639E-2</v>
       </c>
       <c r="H55" s="3">
-        <v>4.3410569917905414E-2</v>
+        <v>1.0201645079494639E-2</v>
       </c>
       <c r="I55" s="3">
-        <v>4.3410569917905414E-2</v>
-      </c>
-      <c r="J55" s="3">
-        <v>4.3410569917905414E-2</v>
-      </c>
-      <c r="K55" s="3">
-        <v>4.3410569917905414E-2</v>
-      </c>
-      <c r="L55" s="3">
-        <v>4.3410569917905414E-2</v>
-      </c>
-      <c r="M55" s="3">
-        <v>4.3410569917905414E-2</v>
-      </c>
-      <c r="N55" s="3">
-        <v>4.3410569917905414E-2</v>
-      </c>
-      <c r="O55" s="3">
-        <v>4.3410569917905414E-2</v>
-      </c>
-    </row>
-    <row r="57" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B57" t="s">
+        <v>1.0201645079494639E-2</v>
+      </c>
+      <c r="J55" s="3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K55" s="3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L55" s="3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="M55" s="3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="N55" s="3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="O55" s="3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="T55">
+        <f t="array" ref="T55:U56">T49:U50*T52:U53</f>
+        <v>6</v>
+      </c>
+      <c r="U55">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="56" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="F56" s="3">
+        <v>-5.1309804294583474E-4</v>
+      </c>
+      <c r="G56" s="3">
+        <v>1.0201645079494639E-2</v>
+      </c>
+      <c r="H56" s="3">
+        <v>1.0201645079494639E-2</v>
+      </c>
+      <c r="I56" s="3">
+        <v>1.0201645079494639E-2</v>
+      </c>
+      <c r="J56" s="3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K56" s="3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L56" s="3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="M56" s="3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="N56" s="3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="O56" s="3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="T56">
+        <v>10</v>
+      </c>
+      <c r="U56">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="57" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="F57" s="3">
+        <v>-5.1309804294583474E-4</v>
+      </c>
+      <c r="G57" s="3">
+        <v>1.0201645079494639E-2</v>
+      </c>
+      <c r="H57" s="3">
+        <v>1.0201645079494639E-2</v>
+      </c>
+      <c r="I57" s="3">
+        <v>1.0201645079494639E-2</v>
+      </c>
+      <c r="J57" s="3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K57" s="3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L57" s="3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="M57" s="3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="N57" s="3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="O57" s="3" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="58" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="F58" s="3">
+        <v>-5.1309804294583474E-4</v>
+      </c>
+      <c r="G58" s="3">
+        <v>1.0201645079494639E-2</v>
+      </c>
+      <c r="H58" s="3">
+        <v>1.0201645079494639E-2</v>
+      </c>
+      <c r="I58" s="3">
+        <v>1.0201645079494639E-2</v>
+      </c>
+      <c r="J58" s="3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K58" s="3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L58" s="3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="M58" s="3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="N58" s="3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="O58" s="3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="S58">
+        <f t="array" ref="S58:V61">S37:V37*S41:V43</f>
+        <v>39</v>
+      </c>
+      <c r="T58">
+        <v>36</v>
+      </c>
+      <c r="U58">
+        <v>14</v>
+      </c>
+      <c r="V58">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="59" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="S59">
+        <v>24</v>
+      </c>
+      <c r="T59">
+        <v>28</v>
+      </c>
+      <c r="U59">
+        <v>8</v>
+      </c>
+      <c r="V59">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="60" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
+        <v>48</v>
+      </c>
+      <c r="F60" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="S60">
+        <v>18</v>
+      </c>
+      <c r="T60">
+        <v>16</v>
+      </c>
+      <c r="U60">
+        <v>0</v>
+      </c>
+      <c r="V60">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="61" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="D61" t="s">
+        <v>51</v>
+      </c>
+      <c r="F61" s="3">
+        <f t="array" ref="F61:I61">Eo*H</f>
+        <v>-1.3590537003052405E-3</v>
+      </c>
+      <c r="G61" s="3">
+        <v>2.7021314318190753E-2</v>
+      </c>
+      <c r="H61" s="3">
+        <v>2.7021314318190753E-2</v>
+      </c>
+      <c r="I61" s="3">
+        <v>2.7021314318190753E-2</v>
+      </c>
+      <c r="S61" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="T61" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="U61" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="V61" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="63" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="S63">
+        <f t="array" ref="S63:V66">Eo*H</f>
+        <v>-1.3590537003052405E-3</v>
+      </c>
+      <c r="T63">
+        <v>2.7021314318190753E-2</v>
+      </c>
+      <c r="U63">
+        <v>2.7021314318190753E-2</v>
+      </c>
+      <c r="V63">
+        <v>2.7021314318190753E-2</v>
+      </c>
+    </row>
+    <row r="64" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="S64">
+        <v>-1.3590537003052405E-3</v>
+      </c>
+      <c r="T64">
+        <v>2.7021314318190753E-2</v>
+      </c>
+      <c r="U64">
+        <v>2.7021314318190753E-2</v>
+      </c>
+      <c r="V64">
+        <v>2.7021314318190753E-2</v>
+      </c>
+    </row>
+    <row r="65" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="S65">
+        <v>-1.3590537003052405E-3</v>
+      </c>
+      <c r="T65">
+        <v>2.7021314318190753E-2</v>
+      </c>
+      <c r="U65">
+        <v>2.7021314318190753E-2</v>
+      </c>
+      <c r="V65">
+        <v>2.7021314318190753E-2</v>
+      </c>
+    </row>
+    <row r="66" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B66" t="s">
         <v>50</v>
       </c>
-      <c r="F57" s="4" t="s">
+      <c r="F66" s="4" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="58" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="D58" t="s">
-        <v>53</v>
-      </c>
-      <c r="F58" s="3">
-        <f t="array" ref="F58:I58">Eo*H</f>
+      <c r="S66">
         <v>-1.3590537003052405E-3</v>
       </c>
-      <c r="G58" s="3">
+      <c r="T66">
         <v>2.7021314318190753E-2</v>
       </c>
-      <c r="H58" s="3">
+      <c r="U66">
         <v>2.7021314318190753E-2</v>
       </c>
-      <c r="I58" s="3">
+      <c r="V66">
         <v>2.7021314318190753E-2</v>
       </c>
     </row>
-    <row r="60" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B60" t="s">
+    <row r="67" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="D67" t="s">
         <v>52</v>
       </c>
-      <c r="F60" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="61" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="D61" t="s">
-        <v>54</v>
-      </c>
-      <c r="F61" s="3">
-        <f t="array" ref="F61:O61">Eh*X</f>
-        <v>0</v>
-      </c>
-      <c r="G61" s="3">
-        <v>0</v>
-      </c>
-      <c r="H61" s="3">
-        <v>0</v>
-      </c>
-      <c r="I61" s="3">
-        <v>0</v>
-      </c>
-      <c r="J61" s="3">
-        <v>0</v>
-      </c>
-      <c r="K61" s="3">
-        <v>0</v>
-      </c>
-      <c r="L61" s="3">
-        <v>0</v>
-      </c>
-      <c r="M61" s="3">
-        <v>0</v>
-      </c>
-      <c r="N61" s="3">
-        <v>0</v>
-      </c>
-      <c r="O61" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="I63" s="4"/>
+      <c r="F67" s="3">
+        <f t="array" ref="F67:O67">Eh*X</f>
+        <v>0</v>
+      </c>
+      <c r="G67" s="3">
+        <v>0</v>
+      </c>
+      <c r="H67" s="3">
+        <v>0</v>
+      </c>
+      <c r="I67" s="3">
+        <v>0</v>
+      </c>
+      <c r="J67" s="3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K67" s="3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L67" s="3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="M67" s="3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="N67" s="3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="O67" s="3" t="e">
+        <v>#N/A</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
still trying to resolve backpropagation
</commit_message>
<xml_diff>
--- a/docs/Book1.xlsx
+++ b/docs/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\georgereimer\Source\Repos\neuralNetwork\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD658A82-8622-4155-A5D9-2A70426DDEBC}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F12CB715-830F-4D33-B4E9-74A7C2A489B3}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4290" yWindow="495" windowWidth="18585" windowHeight="10740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -678,16 +678,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:V67"/>
+  <dimension ref="B2:U67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="R33" sqref="R33:T33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="5" max="5" width="10.7109375" customWidth="1"/>
-    <col min="6" max="6" width="8.5703125" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" customWidth="1"/>
     <col min="7" max="7" width="9.28515625" customWidth="1"/>
     <col min="8" max="8" width="9.5703125" customWidth="1"/>
     <col min="9" max="9" width="11.28515625" customWidth="1"/>
@@ -975,7 +975,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="5:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="5:20" x14ac:dyDescent="0.25">
       <c r="E17" s="2">
         <v>1</v>
       </c>
@@ -989,7 +989,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="5:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="5:20" x14ac:dyDescent="0.25">
       <c r="E18" s="2">
         <v>1</v>
       </c>
@@ -1006,7 +1006,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="5:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="5:20" x14ac:dyDescent="0.25">
       <c r="E19" s="2">
         <v>1</v>
       </c>
@@ -1024,7 +1024,7 @@
         <v>0.23500371220159449</v>
       </c>
     </row>
-    <row r="20" spans="5:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="5:20" x14ac:dyDescent="0.25">
       <c r="E20" s="2">
         <v>1</v>
       </c>
@@ -1042,7 +1042,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="21" spans="5:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="5:20" x14ac:dyDescent="0.25">
       <c r="E21" s="2">
         <v>1</v>
       </c>
@@ -1060,7 +1060,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="22" spans="5:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="5:20" x14ac:dyDescent="0.25">
       <c r="E22" s="2">
         <v>1</v>
       </c>
@@ -1078,12 +1078,12 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="24" spans="5:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="5:20" x14ac:dyDescent="0.25">
       <c r="K24" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="5:18" x14ac:dyDescent="0.25">
+    <row r="25" spans="5:20" x14ac:dyDescent="0.25">
       <c r="K25" s="2">
         <v>0.5</v>
       </c>
@@ -1097,12 +1097,12 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="27" spans="5:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="5:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G27" s="7" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="29" spans="5:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="5:20" x14ac:dyDescent="0.25">
       <c r="E29" t="s">
         <v>27</v>
       </c>
@@ -1116,7 +1116,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="30" spans="5:18" x14ac:dyDescent="0.25">
+    <row r="30" spans="5:20" x14ac:dyDescent="0.25">
       <c r="E30" t="s">
         <v>22</v>
       </c>
@@ -1151,7 +1151,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="5:18" x14ac:dyDescent="0.25">
+    <row r="31" spans="5:20" x14ac:dyDescent="0.25">
       <c r="E31" t="s">
         <v>23</v>
       </c>
@@ -1185,8 +1185,17 @@
       <c r="O31" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="5:18" x14ac:dyDescent="0.25">
+      <c r="R31" s="2">
+        <v>1</v>
+      </c>
+      <c r="S31" s="2">
+        <v>2</v>
+      </c>
+      <c r="T31" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="5:20" x14ac:dyDescent="0.25">
       <c r="E32" t="s">
         <v>24</v>
       </c>
@@ -1220,8 +1229,17 @@
       <c r="O32" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="4:22" x14ac:dyDescent="0.25">
+      <c r="R32" s="2">
+        <v>2</v>
+      </c>
+      <c r="S32" s="2">
+        <v>3</v>
+      </c>
+      <c r="T32" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="4:20" x14ac:dyDescent="0.25">
       <c r="E33" t="s">
         <v>25</v>
       </c>
@@ -1255,13 +1273,23 @@
       <c r="O33" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="4:22" x14ac:dyDescent="0.25">
+      <c r="R33">
+        <f t="array" ref="R33:T33">R31:T31*R32:T33</f>
+        <v>2</v>
+      </c>
+      <c r="S33">
+        <v>6</v>
+      </c>
+      <c r="T33">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34" spans="4:20" x14ac:dyDescent="0.25">
       <c r="E34" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="35" spans="4:22" x14ac:dyDescent="0.25">
+    <row r="35" spans="4:20" x14ac:dyDescent="0.25">
       <c r="F35" s="4" t="s">
         <v>29</v>
       </c>
@@ -1269,7 +1297,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="36" spans="4:22" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:20" x14ac:dyDescent="0.25">
       <c r="F36" s="2">
         <v>0.5</v>
       </c>
@@ -1301,21 +1329,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="37" spans="4:22" x14ac:dyDescent="0.25">
-      <c r="S37">
-        <v>3</v>
-      </c>
-      <c r="T37">
-        <v>4</v>
-      </c>
-      <c r="U37">
-        <v>2</v>
-      </c>
-      <c r="V37">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="38" spans="4:22" x14ac:dyDescent="0.25">
+    <row r="38" spans="4:20" x14ac:dyDescent="0.25">
       <c r="F38" s="4" t="s">
         <v>15</v>
       </c>
@@ -1323,7 +1337,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="39" spans="4:22" x14ac:dyDescent="0.25">
+    <row r="39" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D39" s="8" t="s">
         <v>55</v>
       </c>
@@ -1359,24 +1373,12 @@
         <v>2.9898373248074184</v>
       </c>
     </row>
-    <row r="41" spans="4:22" x14ac:dyDescent="0.25">
+    <row r="41" spans="4:20" x14ac:dyDescent="0.25">
       <c r="F41" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="S41">
-        <v>13</v>
-      </c>
-      <c r="T41">
-        <v>9</v>
-      </c>
-      <c r="U41">
-        <v>7</v>
-      </c>
-      <c r="V41">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="42" spans="4:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D42" t="s">
         <v>38</v>
       </c>
@@ -1420,43 +1422,17 @@
         <f t="shared" si="0"/>
         <v>0.95211289369399577</v>
       </c>
-      <c r="S42">
-        <v>8</v>
-      </c>
-      <c r="T42">
-        <v>7</v>
-      </c>
-      <c r="U42">
-        <v>4</v>
-      </c>
-      <c r="V42">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="43" spans="4:22" x14ac:dyDescent="0.25">
-      <c r="S43">
-        <v>6</v>
-      </c>
-      <c r="T43">
-        <v>4</v>
-      </c>
-      <c r="U43">
-        <v>0</v>
-      </c>
-      <c r="V43">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="44" spans="4:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="4:20" x14ac:dyDescent="0.25">
       <c r="R44" s="4"/>
     </row>
-    <row r="45" spans="4:22" x14ac:dyDescent="0.25">
+    <row r="45" spans="4:20" x14ac:dyDescent="0.25">
       <c r="F45" s="4" t="s">
         <v>41</v>
       </c>
       <c r="R45" s="4"/>
     </row>
-    <row r="46" spans="4:22" x14ac:dyDescent="0.25">
+    <row r="46" spans="4:20" x14ac:dyDescent="0.25">
       <c r="F46" s="3">
         <f t="shared" ref="F46:O46" si="1">1/(1+EXP(-F39))*(1-(1/(1+EXP(-F39))))</f>
         <v>4.5593931355641687E-2</v>
@@ -1497,21 +1473,8 @@
         <f t="shared" si="1"/>
         <v>4.5593931355641687E-2</v>
       </c>
-      <c r="S46">
-        <f t="array" ref="S46:V46">MMULT(S37:U37,S41:V43)</f>
-        <v>83</v>
-      </c>
-      <c r="T46">
-        <v>63</v>
-      </c>
-      <c r="U46">
-        <v>37</v>
-      </c>
-      <c r="V46">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="48" spans="4:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="4:20" x14ac:dyDescent="0.25">
       <c r="F48" s="4" t="s">
         <v>40</v>
       </c>
@@ -1519,7 +1482,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="49" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D49" t="s">
         <v>44</v>
       </c>
@@ -1554,27 +1517,13 @@
       <c r="O49" s="3">
         <v>4.3410569917905414E-2</v>
       </c>
-      <c r="T49">
-        <v>2</v>
-      </c>
-      <c r="U49">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="50" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="T50">
-        <v>2</v>
-      </c>
-      <c r="U50">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="51" spans="2:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="2:15" x14ac:dyDescent="0.25">
       <c r="F51" s="4" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="52" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:15" x14ac:dyDescent="0.25">
       <c r="F52" s="3">
         <f>1/(1+EXP(-K13))*(1-(1/(1+EXP(-K13))))</f>
         <v>0.23500371220159449</v>
@@ -1591,27 +1540,13 @@
         <f t="shared" si="2"/>
         <v>0.23500371220159449</v>
       </c>
-      <c r="T52">
-        <v>3</v>
-      </c>
-      <c r="U52">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="53" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="T53">
-        <v>5</v>
-      </c>
-      <c r="U53">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="54" spans="2:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="54" spans="2:15" x14ac:dyDescent="0.25">
       <c r="F54" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="55" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D55" t="s">
         <v>43</v>
       </c>
@@ -1646,15 +1581,8 @@
       <c r="O55" s="3" t="e">
         <v>#N/A</v>
       </c>
-      <c r="T55">
-        <f t="array" ref="T55:U56">T49:U50*T52:U53</f>
-        <v>6</v>
-      </c>
-      <c r="U55">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="56" spans="2:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="56" spans="2:15" x14ac:dyDescent="0.25">
       <c r="F56" s="3">
         <v>-5.1309804294583474E-4</v>
       </c>
@@ -1685,14 +1613,8 @@
       <c r="O56" s="3" t="e">
         <v>#N/A</v>
       </c>
-      <c r="T56">
-        <v>10</v>
-      </c>
-      <c r="U56">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="57" spans="2:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="57" spans="2:15" x14ac:dyDescent="0.25">
       <c r="F57" s="3">
         <v>-5.1309804294583474E-4</v>
       </c>
@@ -1724,7 +1646,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="58" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:15" x14ac:dyDescent="0.25">
       <c r="F58" s="3">
         <v>-5.1309804294583474E-4</v>
       </c>
@@ -1755,55 +1677,16 @@
       <c r="O58" s="3" t="e">
         <v>#N/A</v>
       </c>
-      <c r="S58">
-        <f t="array" ref="S58:V61">S37:V37*S41:V43</f>
-        <v>39</v>
-      </c>
-      <c r="T58">
-        <v>36</v>
-      </c>
-      <c r="U58">
-        <v>14</v>
-      </c>
-      <c r="V58">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="59" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="S59">
-        <v>24</v>
-      </c>
-      <c r="T59">
-        <v>28</v>
-      </c>
-      <c r="U59">
-        <v>8</v>
-      </c>
-      <c r="V59">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="60" spans="2:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="60" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
         <v>48</v>
       </c>
       <c r="F60" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="S60">
-        <v>18</v>
-      </c>
-      <c r="T60">
-        <v>16</v>
-      </c>
-      <c r="U60">
-        <v>0</v>
-      </c>
-      <c r="V60">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="61" spans="2:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="61" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D61" t="s">
         <v>51</v>
       </c>
@@ -1820,83 +1703,16 @@
       <c r="I61" s="3">
         <v>2.7021314318190753E-2</v>
       </c>
-      <c r="S61" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="T61" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="U61" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="V61" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="63" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="S63">
-        <f t="array" ref="S63:V66">Eo*H</f>
-        <v>-1.3590537003052405E-3</v>
-      </c>
-      <c r="T63">
-        <v>2.7021314318190753E-2</v>
-      </c>
-      <c r="U63">
-        <v>2.7021314318190753E-2</v>
-      </c>
-      <c r="V63">
-        <v>2.7021314318190753E-2</v>
-      </c>
-    </row>
-    <row r="64" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="S64">
-        <v>-1.3590537003052405E-3</v>
-      </c>
-      <c r="T64">
-        <v>2.7021314318190753E-2</v>
-      </c>
-      <c r="U64">
-        <v>2.7021314318190753E-2</v>
-      </c>
-      <c r="V64">
-        <v>2.7021314318190753E-2</v>
-      </c>
-    </row>
-    <row r="65" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="S65">
-        <v>-1.3590537003052405E-3</v>
-      </c>
-      <c r="T65">
-        <v>2.7021314318190753E-2</v>
-      </c>
-      <c r="U65">
-        <v>2.7021314318190753E-2</v>
-      </c>
-      <c r="V65">
-        <v>2.7021314318190753E-2</v>
-      </c>
-    </row>
-    <row r="66" spans="2:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="66" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
         <v>50</v>
       </c>
       <c r="F66" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="S66">
-        <v>-1.3590537003052405E-3</v>
-      </c>
-      <c r="T66">
-        <v>2.7021314318190753E-2</v>
-      </c>
-      <c r="U66">
-        <v>2.7021314318190753E-2</v>
-      </c>
-      <c r="V66">
-        <v>2.7021314318190753E-2</v>
-      </c>
-    </row>
-    <row r="67" spans="2:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="67" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D67" t="s">
         <v>52</v>
       </c>

</xml_diff>

<commit_message>
single training example working
</commit_message>
<xml_diff>
--- a/docs/Book1.xlsx
+++ b/docs/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\georgereimer\Source\Repos\neuralNetwork\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F12CB715-830F-4D33-B4E9-74A7C2A489B3}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEAD3CEE-5020-464D-B812-DBF67C5A30F0}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4290" yWindow="495" windowWidth="18585" windowHeight="10740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,15 +21,14 @@
     <definedName name="A">'activation test data (2)'!$F$54:$H$55</definedName>
     <definedName name="ActivationHidden">'activation test data (2)'!$T$24:$T$24</definedName>
     <definedName name="AX">'activation test data (2)'!#REF!</definedName>
-    <definedName name="BiasDerivativeH">'activation test data (2)'!$R$19:$R$22</definedName>
     <definedName name="BiasDerivativeO">'activation test data (2)'!$R$46:$R$55</definedName>
     <definedName name="BiasH">'activation test data (2)'!$K$25:$N$25</definedName>
     <definedName name="BiasO">'activation test data (2)'!$F$36:$O$36</definedName>
-    <definedName name="dWh">'activation test data (2)'!$F$67:$O$67</definedName>
-    <definedName name="dWo">'activation test data (2)'!$F$67:$I$67+'activation test data (2)'!$F$61:$I$61</definedName>
-    <definedName name="Eh">'activation test data (2)'!$F$55:$O$58</definedName>
+    <definedName name="dWh">'activation test data (2)'!$F$64:$I$73</definedName>
+    <definedName name="dWo">'activation test data (2)'!$F$58:$O$61</definedName>
+    <definedName name="Eh">'activation test data (2)'!$F$55:$I$55</definedName>
     <definedName name="Eo">'activation test data (2)'!$F$49:$O$49</definedName>
-    <definedName name="H">'activation test data (2)'!$R$13:$U$13</definedName>
+    <definedName name="H">'activation test data (2)'!$L$18:$O$18</definedName>
     <definedName name="InputX">'activation test data (2)'!#REF!</definedName>
     <definedName name="Output">'activation test data (2)'!$F$42:$O$42</definedName>
     <definedName name="pies">'activation test data (2)'!$V$34:$Y$36</definedName>
@@ -37,9 +36,9 @@
     <definedName name="Wh">'activation test data (2)'!$E$13:$H$22</definedName>
     <definedName name="Wo">'activation test data (2)'!$F$30:$O$33</definedName>
     <definedName name="X">'activation test data (2)'!$C$4:$L$4</definedName>
-    <definedName name="XX">'activation test data (2)'!$J$69:$J$71</definedName>
+    <definedName name="XX">'activation test data (2)'!#REF!</definedName>
     <definedName name="y">'activation test data (2)'!$C$7:$L$7</definedName>
-    <definedName name="Zh">'activation test data (2)'!$K$13:$N$13</definedName>
+    <definedName name="Zh">'activation test data (2)'!$L$13:$O$13</definedName>
     <definedName name="ZhSigmoidPrime">'activation test data (2)'!$F$52:$I$52</definedName>
     <definedName name="ZhWRONG">'activation test data (2)'!#REF!</definedName>
     <definedName name="Zo">'activation test data (2)'!$F$39:$O$39</definedName>
@@ -60,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="55">
   <si>
     <t>input</t>
   </si>
@@ -104,9 +103,6 @@
     <t>Zh</t>
   </si>
   <si>
-    <t>BiasDerivativeH</t>
-  </si>
-  <si>
     <t>Zo</t>
   </si>
   <si>
@@ -206,21 +202,9 @@
     <t>dWo</t>
   </si>
   <si>
-    <t>cost derivative for output weights</t>
-  </si>
-  <si>
     <t>dWh</t>
   </si>
   <si>
-    <t>cost derivative for hidden weights</t>
-  </si>
-  <si>
-    <t>Eo * H</t>
-  </si>
-  <si>
-    <t>Eh * X</t>
-  </si>
-  <si>
     <t>meaning</t>
   </si>
   <si>
@@ -228,6 +212,18 @@
   </si>
   <si>
     <t>dot(H , Wo )+ BiasO =&gt;</t>
+  </si>
+  <si>
+    <t>BACK PROPAGATION</t>
+  </si>
+  <si>
+    <t>dot(H.T,Eo)</t>
+  </si>
+  <si>
+    <t>dot(X.T,Eh)</t>
+  </si>
+  <si>
+    <t>sigmoidPrime =&gt;</t>
   </si>
 </sst>
 </file>
@@ -678,10 +674,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:U67"/>
+  <dimension ref="B2:R73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="R33" sqref="R33:T33"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q14" sqref="Q14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -712,21 +708,21 @@
     <col min="34" max="34" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:21" ht="21" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:15" ht="21" x14ac:dyDescent="0.35">
       <c r="E2" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="2:21" ht="21" x14ac:dyDescent="0.35">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="2:15" ht="21" x14ac:dyDescent="0.35">
       <c r="C3" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E3" s="5"/>
     </row>
-    <row r="4" spans="2:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4" s="6">
         <v>0</v>
       </c>
@@ -758,16 +754,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E5" s="5"/>
     </row>
-    <row r="6" spans="2:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C6" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E6" s="5"/>
     </row>
-    <row r="7" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
         <v>8</v>
       </c>
@@ -802,9 +798,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -837,51 +833,40 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="2:21" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:15" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B9" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="R10" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="2:21" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
       <c r="F11" t="s">
-        <v>31</v>
-      </c>
-      <c r="K11" t="s">
-        <v>37</v>
-      </c>
-      <c r="R11" t="s">
-        <v>11</v>
-      </c>
-      <c r="T11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="12" spans="2:21" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="L11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
       <c r="E12" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="K12" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12" t="s">
+        <v>20</v>
+      </c>
+      <c r="L12" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="L12" t="s">
-        <v>21</v>
-      </c>
-      <c r="R12" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="S12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="M12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
+        <v>26</v>
+      </c>
       <c r="E13" s="2">
         <v>1</v>
       </c>
@@ -894,14 +879,11 @@
       <c r="H13" s="2">
         <v>1</v>
       </c>
-      <c r="I13" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="K13" s="3">
-        <f t="array" ref="K13:N13">MMULT(X,Wh)+BiasH</f>
-        <v>0.5</v>
+      <c r="J13" s="8" t="s">
+        <v>49</v>
       </c>
       <c r="L13" s="3">
+        <f t="array" ref="L13:O13">MMULT(X,Wh)+BiasH</f>
         <v>0.5</v>
       </c>
       <c r="M13" s="3">
@@ -910,157 +892,178 @@
       <c r="N13" s="3">
         <v>0.5</v>
       </c>
-      <c r="P13" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="R13" s="3">
-        <f>1/(1+EXP(-K13))</f>
-        <v>0.62245933120185459</v>
-      </c>
-      <c r="S13" s="3">
+      <c r="O13" s="3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
+        <v>0</v>
+      </c>
+      <c r="E14" s="2">
+        <v>1</v>
+      </c>
+      <c r="F14" s="2">
+        <v>1</v>
+      </c>
+      <c r="G14" s="2">
+        <v>1</v>
+      </c>
+      <c r="H14" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>22</v>
+      </c>
+      <c r="E15" s="2">
+        <v>1</v>
+      </c>
+      <c r="F15" s="2">
+        <v>1</v>
+      </c>
+      <c r="G15" s="2">
+        <v>1</v>
+      </c>
+      <c r="H15" s="2">
+        <v>1</v>
+      </c>
+      <c r="L15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>23</v>
+      </c>
+      <c r="E16" s="2">
+        <v>1</v>
+      </c>
+      <c r="F16" s="2">
+        <v>1</v>
+      </c>
+      <c r="G16" s="2">
+        <v>1</v>
+      </c>
+      <c r="H16" s="2">
+        <v>1</v>
+      </c>
+      <c r="L16" t="s">
+        <v>11</v>
+      </c>
+      <c r="N16" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>24</v>
+      </c>
+      <c r="E17" s="2">
+        <v>1</v>
+      </c>
+      <c r="F17" s="2">
+        <v>1</v>
+      </c>
+      <c r="G17" s="2">
+        <v>1</v>
+      </c>
+      <c r="H17" s="2">
+        <v>1</v>
+      </c>
+      <c r="L17" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
+        <v>25</v>
+      </c>
+      <c r="E18" s="2">
+        <v>1</v>
+      </c>
+      <c r="F18" s="2">
+        <v>1</v>
+      </c>
+      <c r="G18" s="2">
+        <v>1</v>
+      </c>
+      <c r="H18" s="2">
+        <v>1</v>
+      </c>
+      <c r="J18" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="L18" s="3">
         <f>1/(1+EXP(-L13))</f>
         <v>0.62245933120185459</v>
       </c>
-      <c r="T13" s="3">
+      <c r="M18" s="3">
         <f>1/(1+EXP(-M13))</f>
         <v>0.62245933120185459</v>
       </c>
-      <c r="U13" s="3">
+      <c r="N18" s="3">
         <f>1/(1+EXP(-N13))</f>
         <v>0.62245933120185459</v>
       </c>
-    </row>
-    <row r="14" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="E14" s="2">
-        <v>1</v>
-      </c>
-      <c r="F14" s="2">
-        <v>1</v>
-      </c>
-      <c r="G14" s="2">
-        <v>1</v>
-      </c>
-      <c r="H14" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="E15" s="2">
-        <v>1</v>
-      </c>
-      <c r="F15" s="2">
-        <v>1</v>
-      </c>
-      <c r="G15" s="2">
-        <v>1</v>
-      </c>
-      <c r="H15" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="E16" s="2">
-        <v>1</v>
-      </c>
-      <c r="F16" s="2">
-        <v>1</v>
-      </c>
-      <c r="G16" s="2">
-        <v>1</v>
-      </c>
-      <c r="H16" s="2">
-        <v>1</v>
-      </c>
-      <c r="R16" t="s">
+      <c r="O18" s="3">
+        <f>1/(1+EXP(-O13))</f>
+        <v>0.62245933120185459</v>
+      </c>
+    </row>
+    <row r="19" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="E19" s="2">
+        <v>1</v>
+      </c>
+      <c r="F19" s="2">
+        <v>1</v>
+      </c>
+      <c r="G19" s="2">
+        <v>1</v>
+      </c>
+      <c r="H19" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="E20" s="2">
+        <v>1</v>
+      </c>
+      <c r="F20" s="2">
+        <v>1</v>
+      </c>
+      <c r="G20" s="2">
+        <v>1</v>
+      </c>
+      <c r="H20" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="E21" s="2">
+        <v>1</v>
+      </c>
+      <c r="F21" s="2">
+        <v>1</v>
+      </c>
+      <c r="G21" s="2">
+        <v>1</v>
+      </c>
+      <c r="H21" s="2">
+        <v>1</v>
+      </c>
+      <c r="J21" t="s">
+        <v>54</v>
+      </c>
+      <c r="L21" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="5:20" x14ac:dyDescent="0.25">
-      <c r="E17" s="2">
-        <v>1</v>
-      </c>
-      <c r="F17" s="2">
-        <v>1</v>
-      </c>
-      <c r="G17" s="2">
-        <v>1</v>
-      </c>
-      <c r="H17" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="5:20" x14ac:dyDescent="0.25">
-      <c r="E18" s="2">
-        <v>1</v>
-      </c>
-      <c r="F18" s="2">
-        <v>1</v>
-      </c>
-      <c r="G18" s="2">
-        <v>1</v>
-      </c>
-      <c r="H18" s="2">
-        <v>1</v>
-      </c>
-      <c r="R18" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="19" spans="5:20" x14ac:dyDescent="0.25">
-      <c r="E19" s="2">
-        <v>1</v>
-      </c>
-      <c r="F19" s="2">
-        <v>1</v>
-      </c>
-      <c r="G19" s="2">
-        <v>1</v>
-      </c>
-      <c r="H19" s="2">
-        <v>1</v>
-      </c>
-      <c r="R19" s="3">
-        <f>1/(1+EXP(-K13))*(1-(1/(1+EXP(-K13))))</f>
-        <v>0.23500371220159449</v>
-      </c>
-    </row>
-    <row r="20" spans="5:20" x14ac:dyDescent="0.25">
-      <c r="E20" s="2">
-        <v>1</v>
-      </c>
-      <c r="F20" s="2">
-        <v>1</v>
-      </c>
-      <c r="G20" s="2">
-        <v>1</v>
-      </c>
-      <c r="H20" s="2">
-        <v>1</v>
-      </c>
-      <c r="R20" s="3">
-        <f>1/(1+EXP(-K14))*(1-(1/(1+EXP(-K14))))</f>
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="21" spans="5:20" x14ac:dyDescent="0.25">
-      <c r="E21" s="2">
-        <v>1</v>
-      </c>
-      <c r="F21" s="2">
-        <v>1</v>
-      </c>
-      <c r="G21" s="2">
-        <v>1</v>
-      </c>
-      <c r="H21" s="2">
-        <v>1</v>
-      </c>
-      <c r="R21" s="3">
-        <f>1/(1+EXP(-K15))*(1-(1/(1+EXP(-K15))))</f>
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="22" spans="5:20" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:15" x14ac:dyDescent="0.25">
       <c r="E22" s="2">
         <v>1</v>
       </c>
@@ -1073,17 +1076,13 @@
       <c r="H22" s="2">
         <v>1</v>
       </c>
-      <c r="R22" s="3">
-        <f>1/(1+EXP(-K16))*(1-(1/(1+EXP(-K16))))</f>
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="24" spans="5:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="4:15" x14ac:dyDescent="0.25">
       <c r="K24" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="5:20" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:15" x14ac:dyDescent="0.25">
       <c r="K25" s="2">
         <v>0.5</v>
       </c>
@@ -1097,207 +1096,179 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="27" spans="5:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:15" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G27" s="7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="29" spans="5:20" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="29" spans="4:15" x14ac:dyDescent="0.25">
       <c r="E29" t="s">
+        <v>26</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G29" t="s">
         <v>27</v>
       </c>
-      <c r="F29" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G29" t="s">
+      <c r="J29" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="30" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="E30" t="s">
+        <v>21</v>
+      </c>
+      <c r="F30" s="2">
+        <v>1</v>
+      </c>
+      <c r="G30" s="2">
+        <v>1</v>
+      </c>
+      <c r="H30" s="2">
+        <v>1</v>
+      </c>
+      <c r="I30" s="2">
+        <v>1</v>
+      </c>
+      <c r="J30" s="2">
+        <v>1</v>
+      </c>
+      <c r="K30" s="2">
+        <v>1</v>
+      </c>
+      <c r="L30" s="2">
+        <v>1</v>
+      </c>
+      <c r="M30" s="2">
+        <v>1</v>
+      </c>
+      <c r="N30" s="2">
+        <v>1</v>
+      </c>
+      <c r="O30" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="E31" t="s">
+        <v>22</v>
+      </c>
+      <c r="F31" s="2">
+        <v>1</v>
+      </c>
+      <c r="G31" s="2">
+        <v>1</v>
+      </c>
+      <c r="H31" s="2">
+        <v>1</v>
+      </c>
+      <c r="I31" s="2">
+        <v>1</v>
+      </c>
+      <c r="J31" s="2">
+        <v>1</v>
+      </c>
+      <c r="K31" s="2">
+        <v>1</v>
+      </c>
+      <c r="L31" s="2">
+        <v>1</v>
+      </c>
+      <c r="M31" s="2">
+        <v>1</v>
+      </c>
+      <c r="N31" s="2">
+        <v>1</v>
+      </c>
+      <c r="O31" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="E32" t="s">
+        <v>23</v>
+      </c>
+      <c r="F32" s="2">
+        <v>1</v>
+      </c>
+      <c r="G32" s="2">
+        <v>1</v>
+      </c>
+      <c r="H32" s="2">
+        <v>1</v>
+      </c>
+      <c r="I32" s="2">
+        <v>1</v>
+      </c>
+      <c r="J32" s="2">
+        <v>1</v>
+      </c>
+      <c r="K32" s="2">
+        <v>1</v>
+      </c>
+      <c r="L32" s="2">
+        <v>1</v>
+      </c>
+      <c r="M32" s="2">
+        <v>1</v>
+      </c>
+      <c r="N32" s="2">
+        <v>1</v>
+      </c>
+      <c r="O32" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="E33" t="s">
+        <v>24</v>
+      </c>
+      <c r="F33" s="2">
+        <v>1</v>
+      </c>
+      <c r="G33" s="2">
+        <v>1</v>
+      </c>
+      <c r="H33" s="2">
+        <v>1</v>
+      </c>
+      <c r="I33" s="2">
+        <v>1</v>
+      </c>
+      <c r="J33" s="2">
+        <v>1</v>
+      </c>
+      <c r="K33" s="2">
+        <v>1</v>
+      </c>
+      <c r="L33" s="2">
+        <v>1</v>
+      </c>
+      <c r="M33" s="2">
+        <v>1</v>
+      </c>
+      <c r="N33" s="2">
+        <v>1</v>
+      </c>
+      <c r="O33" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="E34" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="35" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="F35" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="J29" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="30" spans="5:20" x14ac:dyDescent="0.25">
-      <c r="E30" t="s">
-        <v>22</v>
-      </c>
-      <c r="F30" s="2">
-        <v>1</v>
-      </c>
-      <c r="G30" s="2">
-        <v>1</v>
-      </c>
-      <c r="H30" s="2">
-        <v>1</v>
-      </c>
-      <c r="I30" s="2">
-        <v>1</v>
-      </c>
-      <c r="J30" s="2">
-        <v>1</v>
-      </c>
-      <c r="K30" s="2">
-        <v>1</v>
-      </c>
-      <c r="L30" s="2">
-        <v>1</v>
-      </c>
-      <c r="M30" s="2">
-        <v>1</v>
-      </c>
-      <c r="N30" s="2">
-        <v>1</v>
-      </c>
-      <c r="O30" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="5:20" x14ac:dyDescent="0.25">
-      <c r="E31" t="s">
-        <v>23</v>
-      </c>
-      <c r="F31" s="2">
-        <v>1</v>
-      </c>
-      <c r="G31" s="2">
-        <v>1</v>
-      </c>
-      <c r="H31" s="2">
-        <v>1</v>
-      </c>
-      <c r="I31" s="2">
-        <v>1</v>
-      </c>
-      <c r="J31" s="2">
-        <v>1</v>
-      </c>
-      <c r="K31" s="2">
-        <v>1</v>
-      </c>
-      <c r="L31" s="2">
-        <v>1</v>
-      </c>
-      <c r="M31" s="2">
-        <v>1</v>
-      </c>
-      <c r="N31" s="2">
-        <v>1</v>
-      </c>
-      <c r="O31" s="2">
-        <v>1</v>
-      </c>
-      <c r="R31" s="2">
-        <v>1</v>
-      </c>
-      <c r="S31" s="2">
-        <v>2</v>
-      </c>
-      <c r="T31" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="32" spans="5:20" x14ac:dyDescent="0.25">
-      <c r="E32" t="s">
-        <v>24</v>
-      </c>
-      <c r="F32" s="2">
-        <v>1</v>
-      </c>
-      <c r="G32" s="2">
-        <v>1</v>
-      </c>
-      <c r="H32" s="2">
-        <v>1</v>
-      </c>
-      <c r="I32" s="2">
-        <v>1</v>
-      </c>
-      <c r="J32" s="2">
-        <v>1</v>
-      </c>
-      <c r="K32" s="2">
-        <v>1</v>
-      </c>
-      <c r="L32" s="2">
-        <v>1</v>
-      </c>
-      <c r="M32" s="2">
-        <v>1</v>
-      </c>
-      <c r="N32" s="2">
-        <v>1</v>
-      </c>
-      <c r="O32" s="2">
-        <v>1</v>
-      </c>
-      <c r="R32" s="2">
-        <v>2</v>
-      </c>
-      <c r="S32" s="2">
-        <v>3</v>
-      </c>
-      <c r="T32" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="33" spans="4:20" x14ac:dyDescent="0.25">
-      <c r="E33" t="s">
-        <v>25</v>
-      </c>
-      <c r="F33" s="2">
-        <v>1</v>
-      </c>
-      <c r="G33" s="2">
-        <v>1</v>
-      </c>
-      <c r="H33" s="2">
-        <v>1</v>
-      </c>
-      <c r="I33" s="2">
-        <v>1</v>
-      </c>
-      <c r="J33" s="2">
-        <v>1</v>
-      </c>
-      <c r="K33" s="2">
-        <v>1</v>
-      </c>
-      <c r="L33" s="2">
-        <v>1</v>
-      </c>
-      <c r="M33" s="2">
-        <v>1</v>
-      </c>
-      <c r="N33" s="2">
-        <v>1</v>
-      </c>
-      <c r="O33" s="2">
-        <v>1</v>
-      </c>
-      <c r="R33">
-        <f t="array" ref="R33:T33">R31:T31*R32:T33</f>
-        <v>2</v>
-      </c>
-      <c r="S33">
-        <v>6</v>
-      </c>
-      <c r="T33">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="34" spans="4:20" x14ac:dyDescent="0.25">
-      <c r="E34" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="35" spans="4:20" x14ac:dyDescent="0.25">
-      <c r="F35" s="4" t="s">
-        <v>29</v>
-      </c>
       <c r="G35" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="36" spans="4:20" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="36" spans="4:18" x14ac:dyDescent="0.25">
       <c r="F36" s="2">
         <v>0.5</v>
       </c>
@@ -1329,17 +1300,17 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="38" spans="4:20" x14ac:dyDescent="0.25">
+    <row r="38" spans="4:18" x14ac:dyDescent="0.25">
       <c r="F38" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G38" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="39" spans="4:20" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="39" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D39" s="8" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="F39" s="3">
         <f t="array" ref="F39:O39">MMULT(H,Wo)+BiasO</f>
@@ -1373,14 +1344,14 @@
         <v>2.9898373248074184</v>
       </c>
     </row>
-    <row r="41" spans="4:20" x14ac:dyDescent="0.25">
+    <row r="41" spans="4:18" x14ac:dyDescent="0.25">
       <c r="F41" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="42" spans="4:20" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="42" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D42" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F42" s="3">
         <f>1/(1+EXP(-F39))</f>
@@ -1423,16 +1394,18 @@
         <v>0.95211289369399577</v>
       </c>
     </row>
-    <row r="44" spans="4:20" x14ac:dyDescent="0.25">
-      <c r="R44" s="4"/>
-    </row>
-    <row r="45" spans="4:20" x14ac:dyDescent="0.25">
+    <row r="44" spans="4:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G44" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="45" spans="4:18" x14ac:dyDescent="0.25">
       <c r="F45" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="R45" s="4"/>
     </row>
-    <row r="46" spans="4:20" x14ac:dyDescent="0.25">
+    <row r="46" spans="4:18" x14ac:dyDescent="0.25">
       <c r="F46" s="3">
         <f t="shared" ref="F46:O46" si="1">1/(1+EXP(-F39))*(1-(1/(1+EXP(-F39))))</f>
         <v>4.5593931355641687E-2</v>
@@ -1474,17 +1447,17 @@
         <v>4.5593931355641687E-2</v>
       </c>
     </row>
-    <row r="48" spans="4:20" x14ac:dyDescent="0.25">
+    <row r="48" spans="4:18" x14ac:dyDescent="0.25">
       <c r="F48" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H48" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="49" spans="2:15" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="49" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D49" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F49" s="3">
         <f t="array" ref="F49:O49">(Output-y)*ZoSigmoidPrime</f>
@@ -1518,206 +1491,242 @@
         <v>4.3410569917905414E-2</v>
       </c>
     </row>
-    <row r="51" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="51" spans="4:15" x14ac:dyDescent="0.25">
       <c r="F51" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="52" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="F52" s="3">
+        <f>1/(1+EXP(-L13))*(1-(1/(1+EXP(-L13))))</f>
+        <v>0.23500371220159449</v>
+      </c>
+      <c r="G52" s="3">
+        <f>1/(1+EXP(-M13))*(1-(1/(1+EXP(-M13))))</f>
+        <v>0.23500371220159449</v>
+      </c>
+      <c r="H52" s="3">
+        <f>1/(1+EXP(-N13))*(1-(1/(1+EXP(-N13))))</f>
+        <v>0.23500371220159449</v>
+      </c>
+      <c r="I52" s="3">
+        <f>1/(1+EXP(-O13))*(1-(1/(1+EXP(-O13))))</f>
+        <v>0.23500371220159449</v>
+      </c>
+    </row>
+    <row r="54" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="F54" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="55" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="D55" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="52" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="F52" s="3">
-        <f>1/(1+EXP(-K13))*(1-(1/(1+EXP(-K13))))</f>
-        <v>0.23500371220159449</v>
-      </c>
-      <c r="G52" s="3">
-        <f t="shared" ref="G52:I52" si="2">1/(1+EXP(-L13))*(1-(1/(1+EXP(-L13))))</f>
-        <v>0.23500371220159449</v>
-      </c>
-      <c r="H52" s="3">
-        <f t="shared" si="2"/>
-        <v>0.23500371220159449</v>
-      </c>
-      <c r="I52" s="3">
-        <f t="shared" si="2"/>
-        <v>0.23500371220159449</v>
-      </c>
-    </row>
-    <row r="54" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="F54" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="55" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="D55" t="s">
-        <v>43</v>
-      </c>
       <c r="F55" s="3">
-        <f t="array" ref="F55:O58">(Eo*Wo)*ZhSigmoidPrime</f>
-        <v>-5.1309804294583474E-4</v>
+        <f t="array" ref="F55:I55">MMULT(Eo,TRANSPOSE(Wo))*ZhSigmoidPrime</f>
+        <v>9.1301707672505936E-2</v>
       </c>
       <c r="G55" s="3">
-        <v>1.0201645079494639E-2</v>
+        <v>9.1301707672505936E-2</v>
       </c>
       <c r="H55" s="3">
-        <v>1.0201645079494639E-2</v>
+        <v>9.1301707672505936E-2</v>
       </c>
       <c r="I55" s="3">
-        <v>1.0201645079494639E-2</v>
-      </c>
-      <c r="J55" s="3" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="K55" s="3" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="L55" s="3" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="M55" s="3" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="N55" s="3" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="O55" s="3" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="56" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="F56" s="3">
-        <v>-5.1309804294583474E-4</v>
-      </c>
-      <c r="G56" s="3">
-        <v>1.0201645079494639E-2</v>
-      </c>
-      <c r="H56" s="3">
-        <v>1.0201645079494639E-2</v>
-      </c>
-      <c r="I56" s="3">
-        <v>1.0201645079494639E-2</v>
-      </c>
-      <c r="J56" s="3" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="K56" s="3" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="L56" s="3" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="M56" s="3" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="N56" s="3" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="O56" s="3" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="57" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="F57" s="3">
-        <v>-5.1309804294583474E-4</v>
-      </c>
-      <c r="G57" s="3">
-        <v>1.0201645079494639E-2</v>
-      </c>
-      <c r="H57" s="3">
-        <v>1.0201645079494639E-2</v>
-      </c>
-      <c r="I57" s="3">
-        <v>1.0201645079494639E-2</v>
-      </c>
-      <c r="J57" s="3" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="K57" s="3" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="L57" s="3" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="M57" s="3" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="N57" s="3" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="O57" s="3" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="58" spans="2:15" x14ac:dyDescent="0.25">
+        <v>9.1301707672505936E-2</v>
+      </c>
+    </row>
+    <row r="57" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="F57" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="58" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="D58" t="s">
+        <v>52</v>
+      </c>
       <c r="F58" s="3">
-        <v>-5.1309804294583474E-4</v>
+        <f t="array" ref="F58:O61">MMULT(TRANSPOSE(H),Eo)</f>
+        <v>-1.3590537003052405E-3</v>
       </c>
       <c r="G58" s="3">
-        <v>1.0201645079494639E-2</v>
+        <v>2.7021314318190753E-2</v>
       </c>
       <c r="H58" s="3">
-        <v>1.0201645079494639E-2</v>
+        <v>2.7021314318190753E-2</v>
       </c>
       <c r="I58" s="3">
-        <v>1.0201645079494639E-2</v>
-      </c>
-      <c r="J58" s="3" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="K58" s="3" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="L58" s="3" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="M58" s="3" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="N58" s="3" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="O58" s="3" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="60" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B60" t="s">
-        <v>48</v>
-      </c>
-      <c r="F60" s="4" t="s">
+        <v>2.7021314318190753E-2</v>
+      </c>
+      <c r="J58" s="3">
+        <v>2.7021314318190753E-2</v>
+      </c>
+      <c r="K58" s="3">
+        <v>2.7021314318190753E-2</v>
+      </c>
+      <c r="L58" s="3">
+        <v>2.7021314318190753E-2</v>
+      </c>
+      <c r="M58" s="3">
+        <v>2.7021314318190753E-2</v>
+      </c>
+      <c r="N58" s="3">
+        <v>2.7021314318190753E-2</v>
+      </c>
+      <c r="O58" s="3">
+        <v>2.7021314318190753E-2</v>
+      </c>
+    </row>
+    <row r="59" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="F59" s="3">
+        <v>-1.3590537003052405E-3</v>
+      </c>
+      <c r="G59" s="3">
+        <v>2.7021314318190753E-2</v>
+      </c>
+      <c r="H59" s="3">
+        <v>2.7021314318190753E-2</v>
+      </c>
+      <c r="I59" s="3">
+        <v>2.7021314318190753E-2</v>
+      </c>
+      <c r="J59" s="3">
+        <v>2.7021314318190753E-2</v>
+      </c>
+      <c r="K59" s="3">
+        <v>2.7021314318190753E-2</v>
+      </c>
+      <c r="L59" s="3">
+        <v>2.7021314318190753E-2</v>
+      </c>
+      <c r="M59" s="3">
+        <v>2.7021314318190753E-2</v>
+      </c>
+      <c r="N59" s="3">
+        <v>2.7021314318190753E-2</v>
+      </c>
+      <c r="O59" s="3">
+        <v>2.7021314318190753E-2</v>
+      </c>
+    </row>
+    <row r="60" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="F60" s="3">
+        <v>-1.3590537003052405E-3</v>
+      </c>
+      <c r="G60" s="3">
+        <v>2.7021314318190753E-2</v>
+      </c>
+      <c r="H60" s="3">
+        <v>2.7021314318190753E-2</v>
+      </c>
+      <c r="I60" s="3">
+        <v>2.7021314318190753E-2</v>
+      </c>
+      <c r="J60" s="3">
+        <v>2.7021314318190753E-2</v>
+      </c>
+      <c r="K60" s="3">
+        <v>2.7021314318190753E-2</v>
+      </c>
+      <c r="L60" s="3">
+        <v>2.7021314318190753E-2</v>
+      </c>
+      <c r="M60" s="3">
+        <v>2.7021314318190753E-2</v>
+      </c>
+      <c r="N60" s="3">
+        <v>2.7021314318190753E-2</v>
+      </c>
+      <c r="O60" s="3">
+        <v>2.7021314318190753E-2</v>
+      </c>
+    </row>
+    <row r="61" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="F61" s="3">
+        <v>-1.3590537003052405E-3</v>
+      </c>
+      <c r="G61" s="3">
+        <v>2.7021314318190753E-2</v>
+      </c>
+      <c r="H61" s="3">
+        <v>2.7021314318190753E-2</v>
+      </c>
+      <c r="I61" s="3">
+        <v>2.7021314318190753E-2</v>
+      </c>
+      <c r="J61" s="3">
+        <v>2.7021314318190753E-2</v>
+      </c>
+      <c r="K61" s="3">
+        <v>2.7021314318190753E-2</v>
+      </c>
+      <c r="L61" s="3">
+        <v>2.7021314318190753E-2</v>
+      </c>
+      <c r="M61" s="3">
+        <v>2.7021314318190753E-2</v>
+      </c>
+      <c r="N61" s="3">
+        <v>2.7021314318190753E-2</v>
+      </c>
+      <c r="O61" s="3">
+        <v>2.7021314318190753E-2</v>
+      </c>
+    </row>
+    <row r="63" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="F63" s="4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="61" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="D61" t="s">
-        <v>51</v>
-      </c>
-      <c r="F61" s="3">
-        <f t="array" ref="F61:I61">Eo*H</f>
-        <v>-1.3590537003052405E-3</v>
-      </c>
-      <c r="G61" s="3">
-        <v>2.7021314318190753E-2</v>
-      </c>
-      <c r="H61" s="3">
-        <v>2.7021314318190753E-2</v>
-      </c>
-      <c r="I61" s="3">
-        <v>2.7021314318190753E-2</v>
-      </c>
-    </row>
-    <row r="66" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B66" t="s">
-        <v>50</v>
-      </c>
-      <c r="F66" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="67" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="D67" t="s">
-        <v>52</v>
-      </c>
+    <row r="64" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="D64" t="s">
+        <v>53</v>
+      </c>
+      <c r="F64" s="3">
+        <f t="array" ref="F64:I73">MMULT(TRANSPOSE(X),Eh)</f>
+        <v>0</v>
+      </c>
+      <c r="G64" s="3">
+        <v>0</v>
+      </c>
+      <c r="H64" s="3">
+        <v>0</v>
+      </c>
+      <c r="I64" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F65" s="3">
+        <v>0</v>
+      </c>
+      <c r="G65" s="3">
+        <v>0</v>
+      </c>
+      <c r="H65" s="3">
+        <v>0</v>
+      </c>
+      <c r="I65" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F66" s="3">
+        <v>0</v>
+      </c>
+      <c r="G66" s="3">
+        <v>0</v>
+      </c>
+      <c r="H66" s="3">
+        <v>0</v>
+      </c>
+      <c r="I66" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F67" s="3">
-        <f t="array" ref="F67:O67">Eh*X</f>
         <v>0</v>
       </c>
       <c r="G67" s="3">
@@ -1729,23 +1738,89 @@
       <c r="I67" s="3">
         <v>0</v>
       </c>
-      <c r="J67" s="3" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="K67" s="3" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="L67" s="3" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="M67" s="3" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="N67" s="3" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="O67" s="3" t="e">
-        <v>#N/A</v>
+    </row>
+    <row r="68" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F68" s="3">
+        <v>0</v>
+      </c>
+      <c r="G68" s="3">
+        <v>0</v>
+      </c>
+      <c r="H68" s="3">
+        <v>0</v>
+      </c>
+      <c r="I68" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F69" s="3">
+        <v>0</v>
+      </c>
+      <c r="G69" s="3">
+        <v>0</v>
+      </c>
+      <c r="H69" s="3">
+        <v>0</v>
+      </c>
+      <c r="I69" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F70" s="3">
+        <v>0</v>
+      </c>
+      <c r="G70" s="3">
+        <v>0</v>
+      </c>
+      <c r="H70" s="3">
+        <v>0</v>
+      </c>
+      <c r="I70" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F71" s="3">
+        <v>0</v>
+      </c>
+      <c r="G71" s="3">
+        <v>0</v>
+      </c>
+      <c r="H71" s="3">
+        <v>0</v>
+      </c>
+      <c r="I71" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F72" s="3">
+        <v>0</v>
+      </c>
+      <c r="G72" s="3">
+        <v>0</v>
+      </c>
+      <c r="H72" s="3">
+        <v>0</v>
+      </c>
+      <c r="I72" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F73" s="3">
+        <v>0</v>
+      </c>
+      <c r="G73" s="3">
+        <v>0</v>
+      </c>
+      <c r="H73" s="3">
+        <v>0</v>
+      </c>
+      <c r="I73" s="3">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added generic algorithm diagrams
</commit_message>
<xml_diff>
--- a/docs/Book1.xlsx
+++ b/docs/Book1.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\georgereimer\Source\Repos\neuralNetwork\docs\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEAD3CEE-5020-464D-B812-DBF67C5A30F0}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="4290" yWindow="495" windowWidth="18585" windowHeight="10740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4290" yWindow="495" windowWidth="18585" windowHeight="10740" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="activation test data (2)" sheetId="2" r:id="rId1"/>
     <sheet name="activation test data" sheetId="1" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
+    <sheet name="Generic Layer Test" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="A">'activation test data (2)'!$F$54:$H$55</definedName>
@@ -30,6 +24,7 @@
     <definedName name="Eo">'activation test data (2)'!$F$49:$O$49</definedName>
     <definedName name="H">'activation test data (2)'!$L$18:$O$18</definedName>
     <definedName name="InputX">'activation test data (2)'!#REF!</definedName>
+    <definedName name="L0">'Generic Layer Test'!$E$7</definedName>
     <definedName name="Output">'activation test data (2)'!$F$42:$O$42</definedName>
     <definedName name="pies">'activation test data (2)'!$V$34:$Y$36</definedName>
     <definedName name="price">'activation test data (2)'!$V$30:$X$31</definedName>
@@ -44,7 +39,7 @@
     <definedName name="Zo">'activation test data (2)'!$F$39:$O$39</definedName>
     <definedName name="ZoSigmoidPrime">'activation test data (2)'!$F$46:$O$46</definedName>
   </definedNames>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -59,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="71">
   <si>
     <t>input</t>
   </si>
@@ -224,12 +219,60 @@
   </si>
   <si>
     <t>sigmoidPrime =&gt;</t>
+  </si>
+  <si>
+    <t>Layer</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>Input X</t>
+  </si>
+  <si>
+    <t>Target Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Z = L * W</t>
+  </si>
+  <si>
+    <t>Forward</t>
+  </si>
+  <si>
+    <t>Back</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>L = A(Z)</t>
+  </si>
+  <si>
+    <t>C(W)</t>
+  </si>
+  <si>
+    <t>Rate</t>
+  </si>
+  <si>
+    <t>Initial</t>
+  </si>
+  <si>
+    <t>pass 1</t>
+  </si>
+  <si>
+    <t>dW = E * L</t>
+  </si>
+  <si>
+    <t>W -= lr * dW</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
@@ -420,7 +463,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -472,7 +515,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -666,18 +709,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:R73"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q14" sqref="Q14"/>
+    <sheetView topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F46" sqref="F46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1830,7 +1873,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1974,15 +2017,273 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P12" sqref="P12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="3" max="3" width="11.85546875" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="6">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" s="6">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C3" s="6">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C6" t="s">
+        <v>56</v>
+      </c>
+      <c r="D6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="E7" s="3">
+        <f>C1</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>0.51721518182005644</v>
+      </c>
+      <c r="D8" s="3">
+        <f>L0*C8</f>
+        <v>2.0688607272802257</v>
+      </c>
+      <c r="E8" s="3">
+        <f>1/(1+EXP(-D8))</f>
+        <v>0.88783956224387894</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9">
+        <v>0.50109152103123156</v>
+      </c>
+      <c r="D9" s="3">
+        <f>E8*C9</f>
+        <v>0.44488887667648808</v>
+      </c>
+      <c r="E9" s="3">
+        <f>1/(1+EXP(-D9))</f>
+        <v>0.60942333365042256</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>3</v>
+      </c>
+      <c r="C10">
+        <v>0.51720999828656755</v>
+      </c>
+      <c r="D10" s="3">
+        <f>E9*C10</f>
+        <v>0.31519984135312934</v>
+      </c>
+      <c r="E10" s="3">
+        <f>1/(1+EXP(-D10))</f>
+        <v>0.5781539733439891</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>63</v>
+      </c>
+      <c r="D12" t="s">
+        <v>65</v>
+      </c>
+      <c r="E12" t="s">
+        <v>69</v>
+      </c>
+      <c r="F12" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>62</v>
+      </c>
+      <c r="B13">
+        <v>3</v>
+      </c>
+      <c r="C13">
+        <f>(E10-$C$2)*(1/(1+EXP(-E10))*(1-(1/(1+EXP(-E10)))))</f>
+        <v>-1.4784353381213871</v>
+      </c>
+      <c r="D13">
+        <f>C13*C9</f>
+        <v>-0.74083141232556893</v>
+      </c>
+      <c r="E13">
+        <f>C13*E10</f>
+        <v>-0.85476326506704392</v>
+      </c>
+      <c r="F13">
+        <f>C10-$C$3*E13</f>
+        <v>0.52575763093723804</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14">
+        <f>(C13*C10)*(1/(1+EXP(-D9))*(1-(1/(1+EXP(-D9)))))</f>
+        <v>-0.18200973577944565</v>
+      </c>
+      <c r="D14">
+        <f>C14*E8</f>
+        <v>-0.1615954441385471</v>
+      </c>
+      <c r="E14">
+        <f>C14*E9</f>
+        <v>-0.11092097993554235</v>
+      </c>
+      <c r="F14">
+        <f>C19-$C$3*E14</f>
+        <v>0.50110920979935547</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <f>(C14*C9)*(1/(1+EXP(-D8))*(1-(1/(1+EXP(-D8)))))</f>
+        <v>-9.0820912762655786E-3</v>
+      </c>
+      <c r="D15">
+        <f>C15*L0</f>
+        <v>-3.6328365105062314E-2</v>
+      </c>
+      <c r="E15">
+        <f>C15*E8</f>
+        <v>-8.0634399429785827E-3</v>
+      </c>
+      <c r="F15">
+        <f>C8-$C$3*E15</f>
+        <v>0.51729581621948617</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>67</v>
+      </c>
+      <c r="D18" t="s">
+        <v>68</v>
+      </c>
+      <c r="E18">
+        <v>2</v>
+      </c>
+      <c r="F18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C19" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="D19">
+        <v>0.50851784753127982</v>
+      </c>
+      <c r="E19">
+        <v>0.50860039221460152</v>
+      </c>
+      <c r="F19">
+        <v>0.51713063151095084</v>
+      </c>
+      <c r="G19">
+        <v>0.51721518182005644</v>
+      </c>
+    </row>
+    <row r="20" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C20" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="D20">
+        <v>0.50107272564531102</v>
+      </c>
+      <c r="E20">
+        <v>0.50107336469369013</v>
+      </c>
+      <c r="F20">
+        <v>0.50109104405172933</v>
+      </c>
+      <c r="G20">
+        <v>0.50109152103123156</v>
+      </c>
+    </row>
+    <row r="21" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C21" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="D21">
+        <v>0.50008153441100756</v>
+      </c>
+      <c r="E21">
+        <v>0.50859773614299053</v>
+      </c>
+      <c r="F21">
+        <v>0.50868157871043673</v>
+      </c>
+      <c r="G21">
+        <v>0.51720999828656755</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
refactored back propagation ready for calc cost and gradient descent implementation
</commit_message>
<xml_diff>
--- a/docs/Book1.xlsx
+++ b/docs/Book1.xlsx
@@ -1,15 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\georgereimer\Source\Repos\neuralNetwork\docs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39D3D646-4A5E-4381-833C-F3CB3F77919F}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4290" yWindow="495" windowWidth="18585" windowHeight="10740" activeTab="2"/>
+    <workbookView xWindow="4290" yWindow="495" windowWidth="18585" windowHeight="10740" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="activation test data (2)" sheetId="2" r:id="rId1"/>
-    <sheet name="activation test data" sheetId="1" r:id="rId2"/>
-    <sheet name="Generic Layer Test" sheetId="3" r:id="rId3"/>
+    <sheet name="dot vector" sheetId="4" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="5" r:id="rId3"/>
+    <sheet name="activation test data" sheetId="1" r:id="rId4"/>
+    <sheet name="Generic Layer Test" sheetId="3" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="A">'activation test data (2)'!$F$54:$H$55</definedName>
@@ -39,7 +47,7 @@
     <definedName name="Zo">'activation test data (2)'!$F$39:$O$39</definedName>
     <definedName name="ZoSigmoidPrime">'activation test data (2)'!$F$46:$O$46</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -47,6 +55,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -54,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="73">
   <si>
     <t>input</t>
   </si>
@@ -267,12 +276,18 @@
   </si>
   <si>
     <t>W -= lr * dW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       </t>
+  </si>
+  <si>
+    <t>delta/activation.T</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
@@ -389,7 +404,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
@@ -399,6 +414,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="4"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Bad" xfId="4" builtinId="27"/>
@@ -463,7 +479,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -515,7 +531,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -709,18 +725,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:R73"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F46" sqref="F46"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1873,7 +1889,1536 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B07E3BB4-1819-42F0-96B3-5CF12172233D}">
+  <dimension ref="B1:AF43"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
+    <col min="3" max="3" width="12" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1" s="9">
+        <v>3.0860796400000001E-2</v>
+      </c>
+      <c r="D1" s="9">
+        <v>0.99999992900000001</v>
+      </c>
+      <c r="E1" s="9">
+        <v>0.29110551600000001</v>
+      </c>
+      <c r="F1" s="9">
+        <v>9.7974309600000007E-3</v>
+      </c>
+      <c r="G1" s="9">
+        <v>0.99257928100000004</v>
+      </c>
+      <c r="H1" s="9">
+        <v>0.99964503299999996</v>
+      </c>
+      <c r="I1" s="9">
+        <v>2.3392612599999999E-5</v>
+      </c>
+      <c r="J1" s="9">
+        <v>0.99999997200000001</v>
+      </c>
+      <c r="K1" s="9">
+        <v>0.68923073800000001</v>
+      </c>
+      <c r="L1" s="9">
+        <v>1.1313855499999999E-3</v>
+      </c>
+      <c r="M1" s="9">
+        <v>1</v>
+      </c>
+      <c r="N1" s="9">
+        <v>0.98534516100000002</v>
+      </c>
+      <c r="O1" s="9">
+        <v>0.99999856799999998</v>
+      </c>
+      <c r="P1" s="9">
+        <v>1.99987002E-2</v>
+      </c>
+      <c r="Q1" s="9">
+        <v>4.6883573199999998E-7</v>
+      </c>
+      <c r="R1" s="9">
+        <v>4.3857888499999997E-11</v>
+      </c>
+      <c r="S1" s="9">
+        <v>0.99990992300000003</v>
+      </c>
+      <c r="T1" s="9">
+        <v>4.44902978E-4</v>
+      </c>
+      <c r="U1" s="9">
+        <v>0.99999998099999998</v>
+      </c>
+      <c r="V1" s="9">
+        <v>0.98849284199999998</v>
+      </c>
+      <c r="W1" s="9">
+        <v>0.99999999900000003</v>
+      </c>
+      <c r="X1" s="9">
+        <v>0.79504211700000005</v>
+      </c>
+      <c r="Y1" s="9">
+        <v>8.4904714699999997E-7</v>
+      </c>
+      <c r="Z1" s="9">
+        <v>2.52248221E-8</v>
+      </c>
+      <c r="AA1" s="9">
+        <v>1</v>
+      </c>
+      <c r="AB1" s="9">
+        <v>0.95282071000000002</v>
+      </c>
+      <c r="AC1" s="9">
+        <v>0.99999803099999995</v>
+      </c>
+      <c r="AD1" s="9">
+        <v>2.09441071E-4</v>
+      </c>
+      <c r="AE1" s="9">
+        <v>3.1865068200000003E-5</v>
+      </c>
+      <c r="AF1" s="9">
+        <v>2.15829309E-10</v>
+      </c>
+    </row>
+    <row r="2" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="B2">
+        <v>2.77348E-3</v>
+      </c>
+      <c r="C2" s="9">
+        <f>$B2*C$1</f>
+        <v>8.5591801599472009E-5</v>
+      </c>
+      <c r="D2" s="9">
+        <f t="shared" ref="D2:AF10" si="0">$B2*D1</f>
+        <v>2.7734798030829202E-3</v>
+      </c>
+      <c r="E2" s="9">
+        <f t="shared" si="0"/>
+        <v>8.0737532651567999E-4</v>
+      </c>
+      <c r="F2" s="9">
+        <f t="shared" si="0"/>
+        <v>2.7172978818940803E-5</v>
+      </c>
+      <c r="G2" s="9">
+        <f t="shared" si="0"/>
+        <v>2.75289878426788E-3</v>
+      </c>
+      <c r="H2" s="9">
+        <f t="shared" si="0"/>
+        <v>2.7724955061248398E-3</v>
+      </c>
+      <c r="I2" s="9">
+        <f t="shared" si="0"/>
+        <v>6.4878943193848003E-8</v>
+      </c>
+      <c r="J2" s="9">
+        <f t="shared" si="0"/>
+        <v>2.7734799223425601E-3</v>
+      </c>
+      <c r="K2" s="9">
+        <f t="shared" si="0"/>
+        <v>1.91156766722824E-3</v>
+      </c>
+      <c r="L2" s="9">
+        <f t="shared" si="0"/>
+        <v>3.1378751952139999E-6</v>
+      </c>
+      <c r="M2" s="9">
+        <f t="shared" si="0"/>
+        <v>2.77348E-3</v>
+      </c>
+      <c r="N2" s="9">
+        <f t="shared" si="0"/>
+        <v>2.7328350971302802E-3</v>
+      </c>
+      <c r="O2" s="9">
+        <f t="shared" si="0"/>
+        <v>2.77347602837664E-3</v>
+      </c>
+      <c r="P2" s="9">
+        <f t="shared" si="0"/>
+        <v>5.5465995030696E-5</v>
+      </c>
+      <c r="Q2" s="9">
+        <f t="shared" si="0"/>
+        <v>1.30030652598736E-9</v>
+      </c>
+      <c r="R2" s="9">
+        <f t="shared" si="0"/>
+        <v>1.2163897659698E-13</v>
+      </c>
+      <c r="S2" s="9">
+        <f t="shared" si="0"/>
+        <v>2.7732301732420403E-3</v>
+      </c>
+      <c r="T2" s="9">
+        <f t="shared" si="0"/>
+        <v>1.23392951142344E-6</v>
+      </c>
+      <c r="U2" s="9">
+        <f t="shared" si="0"/>
+        <v>2.77347994730388E-3</v>
+      </c>
+      <c r="V2" s="9">
+        <f t="shared" si="0"/>
+        <v>2.7415651274301598E-3</v>
+      </c>
+      <c r="W2" s="9">
+        <f t="shared" si="0"/>
+        <v>2.7734799972265202E-3</v>
+      </c>
+      <c r="X2" s="9">
+        <f t="shared" si="0"/>
+        <v>2.2050334106571601E-3</v>
+      </c>
+      <c r="Y2" s="9">
+        <f t="shared" si="0"/>
+        <v>2.35481528126156E-9</v>
+      </c>
+      <c r="Z2" s="9">
+        <f t="shared" si="0"/>
+        <v>6.9960539597908007E-11</v>
+      </c>
+      <c r="AA2" s="9">
+        <f t="shared" si="0"/>
+        <v>2.77348E-3</v>
+      </c>
+      <c r="AB2" s="9">
+        <f t="shared" si="0"/>
+        <v>2.6426291827707999E-3</v>
+      </c>
+      <c r="AC2" s="9">
+        <f t="shared" si="0"/>
+        <v>2.77347453901788E-3</v>
+      </c>
+      <c r="AD2" s="9">
+        <f t="shared" si="0"/>
+        <v>5.8088062159708001E-7</v>
+      </c>
+      <c r="AE2" s="9">
+        <f t="shared" si="0"/>
+        <v>8.8377129351336008E-8</v>
+      </c>
+      <c r="AF2" s="9">
+        <f t="shared" si="0"/>
+        <v>5.9859827192531999E-13</v>
+      </c>
+    </row>
+    <row r="3" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>4.19396E-3</v>
+      </c>
+      <c r="C3" s="9">
+        <f t="shared" ref="C3:C11" si="1">$B3*C$1</f>
+        <v>1.2942894566974402E-4</v>
+      </c>
+      <c r="D3" s="9">
+        <f t="shared" si="0"/>
+        <v>1.1631863354937644E-5</v>
+      </c>
+      <c r="E3" s="9">
+        <f t="shared" si="0"/>
+        <v>3.3860998243937012E-6</v>
+      </c>
+      <c r="F3" s="9">
+        <f t="shared" si="0"/>
+        <v>1.1396238624748497E-7</v>
+      </c>
+      <c r="G3" s="9">
+        <f t="shared" si="0"/>
+        <v>1.1545547385268118E-5</v>
+      </c>
+      <c r="H3" s="9">
+        <f t="shared" si="0"/>
+        <v>1.1627735252867334E-5</v>
+      </c>
+      <c r="I3" s="9">
+        <f t="shared" si="0"/>
+        <v>2.7209969259727075E-10</v>
+      </c>
+      <c r="J3" s="9">
+        <f t="shared" si="0"/>
+        <v>1.1631863855107804E-5</v>
+      </c>
+      <c r="K3" s="9">
+        <f t="shared" si="0"/>
+        <v>8.0170383336485499E-6</v>
+      </c>
+      <c r="L3" s="9">
+        <f t="shared" si="0"/>
+        <v>1.3160123053719708E-8</v>
+      </c>
+      <c r="M3" s="9">
+        <f t="shared" si="0"/>
+        <v>1.16318641808E-5</v>
+      </c>
+      <c r="N3" s="9">
+        <f t="shared" si="0"/>
+        <v>1.1461401083960511E-5</v>
+      </c>
+      <c r="O3" s="9">
+        <f t="shared" si="0"/>
+        <v>1.1631847523970493E-5</v>
+      </c>
+      <c r="P3" s="9">
+        <f t="shared" si="0"/>
+        <v>2.326221645189378E-7</v>
+      </c>
+      <c r="Q3" s="9">
+        <f t="shared" si="0"/>
+        <v>5.453433557729948E-12</v>
+      </c>
+      <c r="R3" s="9">
+        <f t="shared" si="0"/>
+        <v>5.1014900228867028E-16</v>
+      </c>
+      <c r="S3" s="9">
+        <f t="shared" si="0"/>
+        <v>1.1630816417370187E-5</v>
+      </c>
+      <c r="T3" s="9">
+        <f t="shared" si="0"/>
+        <v>5.1750510137294501E-9</v>
+      </c>
+      <c r="U3" s="9">
+        <f t="shared" si="0"/>
+        <v>1.1631863959794581E-5</v>
+      </c>
+      <c r="V3" s="9">
+        <f t="shared" si="0"/>
+        <v>1.1498014481836993E-5</v>
+      </c>
+      <c r="W3" s="9">
+        <f t="shared" si="0"/>
+        <v>1.1631864169168137E-5</v>
+      </c>
+      <c r="X3" s="9">
+        <f t="shared" si="0"/>
+        <v>9.2478219229597039E-6</v>
+      </c>
+      <c r="Y3" s="9">
+        <f t="shared" si="0"/>
+        <v>9.8760010969997329E-12</v>
+      </c>
+      <c r="Z3" s="9">
+        <f t="shared" si="0"/>
+        <v>2.9341170465204229E-13</v>
+      </c>
+      <c r="AA3" s="9">
+        <f t="shared" si="0"/>
+        <v>1.16318641808E-5</v>
+      </c>
+      <c r="AB3" s="9">
+        <f t="shared" si="0"/>
+        <v>1.1083081087373424E-5</v>
+      </c>
+      <c r="AC3" s="9">
+        <f t="shared" si="0"/>
+        <v>1.1631841277659428E-5</v>
+      </c>
+      <c r="AD3" s="9">
+        <f t="shared" si="0"/>
+        <v>2.4361900917532898E-9</v>
+      </c>
+      <c r="AE3" s="9">
+        <f t="shared" si="0"/>
+        <v>3.7065014541432917E-10</v>
+      </c>
+      <c r="AF3" s="9">
+        <f t="shared" si="0"/>
+        <v>2.5104972085239152E-15</v>
+      </c>
+    </row>
+    <row r="4" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>1.23175E-3</v>
+      </c>
+      <c r="C4" s="9">
+        <f t="shared" si="1"/>
+        <v>3.8012785965700002E-5</v>
+      </c>
+      <c r="D4" s="9">
+        <f t="shared" si="0"/>
+        <v>1.4327547687444443E-8</v>
+      </c>
+      <c r="E4" s="9">
+        <f t="shared" si="0"/>
+        <v>4.1708284586969411E-9</v>
+      </c>
+      <c r="F4" s="9">
+        <f t="shared" si="0"/>
+        <v>1.403731692603396E-10</v>
+      </c>
+      <c r="G4" s="9">
+        <f t="shared" si="0"/>
+        <v>1.4221227991804005E-8</v>
+      </c>
+      <c r="H4" s="9">
+        <f t="shared" si="0"/>
+        <v>1.4322462897719338E-8</v>
+      </c>
+      <c r="I4" s="9">
+        <f t="shared" si="0"/>
+        <v>3.3515879635668826E-13</v>
+      </c>
+      <c r="J4" s="9">
+        <f t="shared" si="0"/>
+        <v>1.4327548303529038E-8</v>
+      </c>
+      <c r="K4" s="9">
+        <f t="shared" si="0"/>
+        <v>9.8749869674716021E-9</v>
+      </c>
+      <c r="L4" s="9">
+        <f t="shared" si="0"/>
+        <v>1.6209981571419249E-11</v>
+      </c>
+      <c r="M4" s="9">
+        <f t="shared" si="0"/>
+        <v>1.43275487047004E-8</v>
+      </c>
+      <c r="N4" s="9">
+        <f t="shared" si="0"/>
+        <v>1.4117580785168359E-8</v>
+      </c>
+      <c r="O4" s="9">
+        <f t="shared" si="0"/>
+        <v>1.4327528187650654E-8</v>
+      </c>
+      <c r="P4" s="9">
+        <f t="shared" si="0"/>
+        <v>2.8653235114620165E-10</v>
+      </c>
+      <c r="Q4" s="9">
+        <f t="shared" si="0"/>
+        <v>6.7172667847338637E-15</v>
+      </c>
+      <c r="R4" s="9">
+        <f t="shared" si="0"/>
+        <v>6.2837603356906961E-19</v>
+      </c>
+      <c r="S4" s="9">
+        <f t="shared" si="0"/>
+        <v>1.4326258122095728E-8</v>
+      </c>
+      <c r="T4" s="9">
+        <f t="shared" si="0"/>
+        <v>6.3743690861612497E-12</v>
+      </c>
+      <c r="U4" s="9">
+        <f t="shared" si="0"/>
+        <v>1.4327548432476975E-8</v>
+      </c>
+      <c r="V4" s="9">
+        <f t="shared" si="0"/>
+        <v>1.4162679338002717E-8</v>
+      </c>
+      <c r="W4" s="9">
+        <f t="shared" si="0"/>
+        <v>1.4327548690372853E-8</v>
+      </c>
+      <c r="X4" s="9">
+        <f t="shared" si="0"/>
+        <v>1.1391004653605616E-8</v>
+      </c>
+      <c r="Y4" s="9">
+        <f t="shared" si="0"/>
+        <v>1.216476435122942E-14</v>
+      </c>
+      <c r="Z4" s="9">
+        <f t="shared" si="0"/>
+        <v>3.6140986720515309E-16</v>
+      </c>
+      <c r="AA4" s="9">
+        <f t="shared" si="0"/>
+        <v>1.43275487047004E-8</v>
+      </c>
+      <c r="AB4" s="9">
+        <f t="shared" si="0"/>
+        <v>1.3651585129372215E-8</v>
+      </c>
+      <c r="AC4" s="9">
+        <f t="shared" si="0"/>
+        <v>1.4327520493757E-8</v>
+      </c>
+      <c r="AD4" s="9">
+        <f t="shared" si="0"/>
+        <v>3.0007771455171145E-12</v>
+      </c>
+      <c r="AE4" s="9">
+        <f t="shared" si="0"/>
+        <v>4.5654831661409995E-13</v>
+      </c>
+      <c r="AF4" s="9">
+        <f t="shared" si="0"/>
+        <v>3.0923049365993326E-18</v>
+      </c>
+    </row>
+    <row r="5" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>0.10832103999999999</v>
+      </c>
+      <c r="C5" s="9">
+        <f t="shared" si="1"/>
+        <v>3.3428735612762561E-3</v>
+      </c>
+      <c r="D5" s="9">
+        <f t="shared" si="0"/>
+        <v>1.5519748661535768E-9</v>
+      </c>
+      <c r="E5" s="9">
+        <f t="shared" si="0"/>
+        <v>4.5178847630764969E-10</v>
+      </c>
+      <c r="F5" s="9">
+        <f t="shared" si="0"/>
+        <v>1.5205367682376015E-11</v>
+      </c>
+      <c r="G5" s="9">
+        <f t="shared" si="0"/>
+        <v>1.5404582061493212E-9</v>
+      </c>
+      <c r="H5" s="9">
+        <f t="shared" si="0"/>
+        <v>1.5514240764423723E-9</v>
+      </c>
+      <c r="I5" s="9">
+        <f t="shared" si="0"/>
+        <v>3.6304749386504683E-14</v>
+      </c>
+      <c r="J5" s="9">
+        <f t="shared" si="0"/>
+        <v>1.5519749328885011E-9</v>
+      </c>
+      <c r="K5" s="9">
+        <f t="shared" si="0"/>
+        <v>1.0696688583029701E-9</v>
+      </c>
+      <c r="L5" s="9">
+        <f t="shared" si="0"/>
+        <v>1.7558820621969673E-12</v>
+      </c>
+      <c r="M5" s="9">
+        <f t="shared" si="0"/>
+        <v>1.5519749763438001E-9</v>
+      </c>
+      <c r="N5" s="9">
+        <f t="shared" si="0"/>
+        <v>1.5292310329334531E-9</v>
+      </c>
+      <c r="O5" s="9">
+        <f t="shared" si="0"/>
+        <v>1.551972753915634E-9</v>
+      </c>
+      <c r="P5" s="9">
+        <f t="shared" si="0"/>
+        <v>3.103748226980175E-11</v>
+      </c>
+      <c r="Q5" s="9">
+        <f t="shared" si="0"/>
+        <v>7.276213240798282E-16</v>
+      </c>
+      <c r="R5" s="9">
+        <f t="shared" si="0"/>
+        <v>6.8066345467276522E-20</v>
+      </c>
+      <c r="S5" s="9">
+        <f t="shared" si="0"/>
+        <v>1.551835179093856E-9</v>
+      </c>
+      <c r="T5" s="9">
+        <f t="shared" si="0"/>
+        <v>6.9047828875683614E-13</v>
+      </c>
+      <c r="U5" s="9">
+        <f t="shared" si="0"/>
+        <v>1.5519749468562756E-9</v>
+      </c>
+      <c r="V5" s="9">
+        <f t="shared" si="0"/>
+        <v>1.5341161550789658E-9</v>
+      </c>
+      <c r="W5" s="9">
+        <f t="shared" si="0"/>
+        <v>1.5519749747918252E-9</v>
+      </c>
+      <c r="X5" s="9">
+        <f t="shared" si="0"/>
+        <v>1.2338854707233999E-9</v>
+      </c>
+      <c r="Y5" s="9">
+        <f t="shared" si="0"/>
+        <v>1.3176999258800959E-15</v>
+      </c>
+      <c r="Z5" s="9">
+        <f t="shared" si="0"/>
+        <v>3.9148292681924074E-17</v>
+      </c>
+      <c r="AA5" s="9">
+        <f t="shared" si="0"/>
+        <v>1.5519749763438001E-9</v>
+      </c>
+      <c r="AB5" s="9">
+        <f t="shared" si="0"/>
+        <v>1.4787538988621327E-9</v>
+      </c>
+      <c r="AC5" s="9">
+        <f t="shared" si="0"/>
+        <v>1.5519719205050718E-9</v>
+      </c>
+      <c r="AD5" s="9">
+        <f t="shared" si="0"/>
+        <v>3.2504730121064514E-13</v>
+      </c>
+      <c r="AE5" s="9">
+        <f t="shared" si="0"/>
+        <v>4.9453788465888584E-14</v>
+      </c>
+      <c r="AF5" s="9">
+        <f t="shared" si="0"/>
+        <v>3.3496168672957373E-19</v>
+      </c>
+    </row>
+    <row r="6" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>-8.0462000000000003E-4</v>
+      </c>
+      <c r="C6" s="9">
+        <f t="shared" si="1"/>
+        <v>-2.4831213999368004E-5</v>
+      </c>
+      <c r="D6" s="9">
+        <f t="shared" si="0"/>
+        <v>-1.2487500168044911E-12</v>
+      </c>
+      <c r="E6" s="9">
+        <f t="shared" si="0"/>
+        <v>-3.635180438066611E-13</v>
+      </c>
+      <c r="F6" s="9">
+        <f t="shared" si="0"/>
+        <v>-1.223454294459339E-14</v>
+      </c>
+      <c r="G6" s="9">
+        <f t="shared" si="0"/>
+        <v>-1.2394834818318669E-12</v>
+      </c>
+      <c r="H6" s="9">
+        <f t="shared" si="0"/>
+        <v>-1.2483068403870616E-12</v>
+      </c>
+      <c r="I6" s="9">
+        <f t="shared" si="0"/>
+        <v>-2.92115274513694E-17</v>
+      </c>
+      <c r="J6" s="9">
+        <f t="shared" si="0"/>
+        <v>-1.2487500705007457E-12</v>
+      </c>
+      <c r="K6" s="9">
+        <f t="shared" si="0"/>
+        <v>-8.6067695676773578E-13</v>
+      </c>
+      <c r="L6" s="9">
+        <f t="shared" si="0"/>
+        <v>-1.4128178248849239E-15</v>
+      </c>
+      <c r="M6" s="9">
+        <f t="shared" si="0"/>
+        <v>-1.2487501054657485E-12</v>
+      </c>
+      <c r="N6" s="9">
+        <f t="shared" si="0"/>
+        <v>-1.2304498737189151E-12</v>
+      </c>
+      <c r="O6" s="9">
+        <f t="shared" si="0"/>
+        <v>-1.2487483172555974E-12</v>
+      </c>
+      <c r="P6" s="9">
+        <f t="shared" si="0"/>
+        <v>-2.4973378983927884E-14</v>
+      </c>
+      <c r="Q6" s="9">
+        <f t="shared" si="0"/>
+        <v>-5.8545866978111135E-19</v>
+      </c>
+      <c r="R6" s="9">
+        <f t="shared" si="0"/>
+        <v>-5.4767542889880033E-23</v>
+      </c>
+      <c r="S6" s="9">
+        <f t="shared" si="0"/>
+        <v>-1.2486376218024985E-12</v>
+      </c>
+      <c r="T6" s="9">
+        <f t="shared" si="0"/>
+        <v>-5.5557264069952555E-16</v>
+      </c>
+      <c r="U6" s="9">
+        <f t="shared" si="0"/>
+        <v>-1.2487500817394964E-12</v>
+      </c>
+      <c r="V6" s="9">
+        <f t="shared" si="0"/>
+        <v>-1.2343805406996375E-12</v>
+      </c>
+      <c r="W6" s="9">
+        <f t="shared" si="0"/>
+        <v>-1.2487501042169984E-12</v>
+      </c>
+      <c r="X6" s="9">
+        <f t="shared" si="0"/>
+        <v>-9.92808927453462E-13</v>
+      </c>
+      <c r="Y6" s="9">
+        <f t="shared" si="0"/>
+        <v>-1.0602477143616428E-18</v>
+      </c>
+      <c r="Z6" s="9">
+        <f t="shared" si="0"/>
+        <v>-3.1499499257729749E-20</v>
+      </c>
+      <c r="AA6" s="9">
+        <f t="shared" si="0"/>
+        <v>-1.2487501054657485E-12</v>
+      </c>
+      <c r="AB6" s="9">
+        <f t="shared" si="0"/>
+        <v>-1.1898349621024493E-12</v>
+      </c>
+      <c r="AC6" s="9">
+        <f t="shared" si="0"/>
+        <v>-1.2487476466767909E-12</v>
+      </c>
+      <c r="AD6" s="9">
+        <f t="shared" si="0"/>
+        <v>-2.6153955950010928E-16</v>
+      </c>
+      <c r="AE6" s="9">
+        <f t="shared" si="0"/>
+        <v>-3.9791507275423276E-17</v>
+      </c>
+      <c r="AF6" s="9">
+        <f t="shared" si="0"/>
+        <v>-2.6951687237634964E-22</v>
+      </c>
+    </row>
+    <row r="7" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>6.6705399999999998E-2</v>
+      </c>
+      <c r="C7" s="9">
+        <f t="shared" si="1"/>
+        <v>2.0585817681805598E-3</v>
+      </c>
+      <c r="D7" s="9">
+        <f t="shared" si="0"/>
+        <v>-8.3298369370950297E-14</v>
+      </c>
+      <c r="E7" s="9">
+        <f t="shared" si="0"/>
+        <v>-2.4248616519340851E-14</v>
+      </c>
+      <c r="F7" s="9">
+        <f t="shared" si="0"/>
+        <v>-8.1611008093627993E-16</v>
+      </c>
+      <c r="G7" s="9">
+        <f t="shared" si="0"/>
+        <v>-8.2680241448987412E-14</v>
+      </c>
+      <c r="H7" s="9">
+        <f t="shared" si="0"/>
+        <v>-8.3268807110755101E-14</v>
+      </c>
+      <c r="I7" s="9">
+        <f t="shared" si="0"/>
+        <v>-1.9485666232545764E-18</v>
+      </c>
+      <c r="J7" s="9">
+        <f t="shared" si="0"/>
+        <v>-8.3298372952780445E-14</v>
+      </c>
+      <c r="K7" s="9">
+        <f t="shared" si="0"/>
+        <v>-5.7411800671974523E-14</v>
+      </c>
+      <c r="L7" s="9">
+        <f t="shared" si="0"/>
+        <v>-9.4242578136078795E-17</v>
+      </c>
+      <c r="M7" s="9">
+        <f t="shared" si="0"/>
+        <v>-8.329837528513494E-14</v>
+      </c>
+      <c r="N7" s="9">
+        <f t="shared" si="0"/>
+        <v>-8.207765100636972E-14</v>
+      </c>
+      <c r="O7" s="9">
+        <f t="shared" si="0"/>
+        <v>-8.3298256001861529E-14</v>
+      </c>
+      <c r="P7" s="9">
+        <f t="shared" si="0"/>
+        <v>-1.665859234474503E-15</v>
+      </c>
+      <c r="Q7" s="9">
+        <f t="shared" si="0"/>
+        <v>-3.9053254751216943E-20</v>
+      </c>
+      <c r="R7" s="9">
+        <f t="shared" si="0"/>
+        <v>-3.6532908554866032E-24</v>
+      </c>
+      <c r="S7" s="9">
+        <f t="shared" si="0"/>
+        <v>-8.3290872017384385E-14</v>
+      </c>
+      <c r="T7" s="9">
+        <f t="shared" si="0"/>
+        <v>-3.705969522691813E-17</v>
+      </c>
+      <c r="U7" s="9">
+        <f t="shared" si="0"/>
+        <v>-8.3298373702465798E-14</v>
+      </c>
+      <c r="V7" s="9">
+        <f t="shared" si="0"/>
+        <v>-8.2339847719585603E-14</v>
+      </c>
+      <c r="W7" s="9">
+        <f t="shared" si="0"/>
+        <v>-8.3298375201836567E-14</v>
+      </c>
+      <c r="X7" s="9">
+        <f t="shared" si="0"/>
+        <v>-6.6225716629354165E-14</v>
+      </c>
+      <c r="Y7" s="9">
+        <f t="shared" si="0"/>
+        <v>-7.0724247885579129E-20</v>
+      </c>
+      <c r="Z7" s="9">
+        <f t="shared" si="0"/>
+        <v>-2.1011866977865661E-21</v>
+      </c>
+      <c r="AA7" s="9">
+        <f t="shared" si="0"/>
+        <v>-8.329837528513494E-14</v>
+      </c>
+      <c r="AB7" s="9">
+        <f t="shared" si="0"/>
+        <v>-7.936841708102872E-14</v>
+      </c>
+      <c r="AC7" s="9">
+        <f t="shared" si="0"/>
+        <v>-8.3298211270634002E-14</v>
+      </c>
+      <c r="AD7" s="9">
+        <f t="shared" si="0"/>
+        <v>-1.744610093227859E-17</v>
+      </c>
+      <c r="AE7" s="9">
+        <f t="shared" si="0"/>
+        <v>-2.6543084094100196E-18</v>
+      </c>
+      <c r="AF7" s="9">
+        <f t="shared" si="0"/>
+        <v>-1.7978230778613352E-23</v>
+      </c>
+    </row>
+    <row r="8" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="B8" s="9">
+        <v>9.0112819000000001E-5</v>
+      </c>
+      <c r="C8" s="9">
+        <f t="shared" si="1"/>
+        <v>2.7809533601890518E-6</v>
+      </c>
+      <c r="D8" s="9">
+        <f t="shared" si="0"/>
+        <v>-7.5062508821195881E-18</v>
+      </c>
+      <c r="E8" s="9">
+        <f t="shared" si="0"/>
+        <v>-2.1851111914077722E-18</v>
+      </c>
+      <c r="F8" s="9">
+        <f t="shared" si="0"/>
+        <v>-7.3541980007486343E-20</v>
+      </c>
+      <c r="G8" s="9">
+        <f t="shared" si="0"/>
+        <v>-7.4505496325689012E-18</v>
+      </c>
+      <c r="H8" s="9">
+        <f t="shared" si="0"/>
+        <v>-7.5035869435173875E-18</v>
+      </c>
+      <c r="I8" s="9">
+        <f t="shared" si="0"/>
+        <v>-1.7559083143078083E-22</v>
+      </c>
+      <c r="J8" s="9">
+        <f t="shared" si="0"/>
+        <v>-7.5062512048884E-18</v>
+      </c>
+      <c r="K8" s="9">
+        <f t="shared" si="0"/>
+        <v>-5.173539202417719E-18</v>
+      </c>
+      <c r="L8" s="9">
+        <f t="shared" si="0"/>
+        <v>-8.4924643856698263E-21</v>
+      </c>
+      <c r="M8" s="9">
+        <f t="shared" si="0"/>
+        <v>-7.5062514150634385E-18</v>
+      </c>
+      <c r="N8" s="9">
+        <f t="shared" si="0"/>
+        <v>-7.3962485090821627E-18</v>
+      </c>
+      <c r="O8" s="9">
+        <f t="shared" si="0"/>
+        <v>-7.5062406661114119E-18</v>
+      </c>
+      <c r="P8" s="9">
+        <f t="shared" si="0"/>
+        <v>-1.5011527167567946E-19</v>
+      </c>
+      <c r="Q8" s="9">
+        <f t="shared" si="0"/>
+        <v>-3.5191988767573028E-24</v>
+      </c>
+      <c r="R8" s="9">
+        <f t="shared" si="0"/>
+        <v>-3.2920833761481944E-28</v>
+      </c>
+      <c r="S8" s="9">
+        <f t="shared" si="0"/>
+        <v>-7.5055752744547247E-18</v>
+      </c>
+      <c r="T8" s="9">
+        <f t="shared" si="0"/>
+        <v>-3.3395536081784373E-21</v>
+      </c>
+      <c r="U8" s="9">
+        <f t="shared" si="0"/>
+        <v>-7.5062512724446606E-18</v>
+      </c>
+      <c r="V8" s="9">
+        <f t="shared" si="0"/>
+        <v>-7.4198757940425796E-18</v>
+      </c>
+      <c r="W8" s="9">
+        <f t="shared" si="0"/>
+        <v>-7.5062514075571866E-18</v>
+      </c>
+      <c r="X8" s="9">
+        <f t="shared" si="0"/>
+        <v>-5.9677860157662817E-18</v>
+      </c>
+      <c r="Y8" s="9">
+        <f t="shared" si="0"/>
+        <v>-6.3731613486243248E-24</v>
+      </c>
+      <c r="Z8" s="9">
+        <f t="shared" si="0"/>
+        <v>-1.8934385658284853E-25</v>
+      </c>
+      <c r="AA8" s="9">
+        <f t="shared" si="0"/>
+        <v>-7.5062514150634385E-18</v>
+      </c>
+      <c r="AB8" s="9">
+        <f t="shared" si="0"/>
+        <v>-7.1521118027392487E-18</v>
+      </c>
+      <c r="AC8" s="9">
+        <f t="shared" si="0"/>
+        <v>-7.5062366352544016E-18</v>
+      </c>
+      <c r="AD8" s="9">
+        <f t="shared" si="0"/>
+        <v>-1.5721173355661518E-21</v>
+      </c>
+      <c r="AE8" s="9">
+        <f t="shared" si="0"/>
+        <v>-2.3918721326734299E-22</v>
+      </c>
+      <c r="AF8" s="9">
+        <f t="shared" si="0"/>
+        <v>-1.620069056093414E-27</v>
+      </c>
+    </row>
+    <row r="9" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="B9" s="9">
+        <v>2.6792646800000001E-6</v>
+      </c>
+      <c r="C9" s="9">
+        <f t="shared" si="1"/>
+        <v>8.2684241791191164E-8</v>
+      </c>
+      <c r="D9" s="9">
+        <f t="shared" si="0"/>
+        <v>-2.0111232867681857E-23</v>
+      </c>
+      <c r="E9" s="9">
+        <f t="shared" si="0"/>
+        <v>-5.8544912370115635E-24</v>
+      </c>
+      <c r="F9" s="9">
+        <f t="shared" si="0"/>
+        <v>-1.9703842953132429E-25</v>
+      </c>
+      <c r="G9" s="9">
+        <f t="shared" si="0"/>
+        <v>-1.9961994477128837E-23</v>
+      </c>
+      <c r="H9" s="9">
+        <f t="shared" si="0"/>
+        <v>-2.0104095471075293E-23</v>
+      </c>
+      <c r="I9" s="9">
+        <f t="shared" si="0"/>
+        <v>-4.7045431278432492E-28</v>
+      </c>
+      <c r="J9" s="9">
+        <f t="shared" si="0"/>
+        <v>-2.0111233732464936E-23</v>
+      </c>
+      <c r="K9" s="9">
+        <f t="shared" si="0"/>
+        <v>-1.3861280855633166E-23</v>
+      </c>
+      <c r="L9" s="9">
+        <f t="shared" si="0"/>
+        <v>-2.2753559874683065E-26</v>
+      </c>
+      <c r="M9" s="9">
+        <f t="shared" si="0"/>
+        <v>-2.0111234295579492E-23</v>
+      </c>
+      <c r="N9" s="9">
+        <f t="shared" si="0"/>
+        <v>-1.9816507394886499E-23</v>
+      </c>
+      <c r="O9" s="9">
+        <f t="shared" si="0"/>
+        <v>-2.011120549629198E-23</v>
+      </c>
+      <c r="P9" s="9">
+        <f t="shared" si="0"/>
+        <v>-4.0219854532925238E-25</v>
+      </c>
+      <c r="Q9" s="9">
+        <f t="shared" si="0"/>
+        <v>-9.4288652523915151E-30</v>
+      </c>
+      <c r="R9" s="9">
+        <f t="shared" si="0"/>
+        <v>-8.8203627133290127E-34</v>
+      </c>
+      <c r="S9" s="9">
+        <f t="shared" si="0"/>
+        <v>-2.010942273592785E-23</v>
+      </c>
+      <c r="T9" s="9">
+        <f t="shared" si="0"/>
+        <v>-8.9475480293590472E-27</v>
+      </c>
+      <c r="U9" s="9">
+        <f t="shared" si="0"/>
+        <v>-2.0111233913466036E-23</v>
+      </c>
+      <c r="V9" s="9">
+        <f t="shared" si="0"/>
+        <v>-1.9879811144965238E-23</v>
+      </c>
+      <c r="W9" s="9">
+        <f t="shared" si="0"/>
+        <v>-2.0111234275468256E-23</v>
+      </c>
+      <c r="X9" s="9">
+        <f t="shared" si="0"/>
+        <v>-1.5989278289840522E-23</v>
+      </c>
+      <c r="Y9" s="9">
+        <f t="shared" si="0"/>
+        <v>-1.7075386101310321E-29</v>
+      </c>
+      <c r="Z9" s="9">
+        <f t="shared" si="0"/>
+        <v>-5.073023073174116E-31</v>
+      </c>
+      <c r="AA9" s="9">
+        <f t="shared" si="0"/>
+        <v>-2.0111234295579492E-23</v>
+      </c>
+      <c r="AB9" s="9">
+        <f t="shared" si="0"/>
+        <v>-1.9162400540490398E-23</v>
+      </c>
+      <c r="AC9" s="9">
+        <f t="shared" si="0"/>
+        <v>-2.0111194696559161E-23</v>
+      </c>
+      <c r="AD9" s="9">
+        <f t="shared" si="0"/>
+        <v>-4.2121184499980984E-27</v>
+      </c>
+      <c r="AE9" s="9">
+        <f t="shared" si="0"/>
+        <v>-6.4084585241481949E-28</v>
+      </c>
+      <c r="AF9" s="9">
+        <f t="shared" si="0"/>
+        <v>-4.3405938011520228E-33</v>
+      </c>
+    </row>
+    <row r="10" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>2.182688E-2</v>
+      </c>
+      <c r="C10" s="9">
+        <f t="shared" si="1"/>
+        <v>6.7359489972723197E-4</v>
+      </c>
+      <c r="D10" s="9">
+        <f t="shared" si="0"/>
+        <v>-4.3896546645494776E-25</v>
+      </c>
+      <c r="E10" s="9">
+        <f t="shared" si="0"/>
+        <v>-1.2778527769130294E-25</v>
+      </c>
+      <c r="F10" s="9">
+        <f t="shared" si="0"/>
+        <v>-4.3007341567686715E-27</v>
+      </c>
+      <c r="G10" s="9">
+        <f t="shared" si="0"/>
+        <v>-4.3570805801295384E-25</v>
+      </c>
+      <c r="H10" s="9">
+        <f t="shared" si="0"/>
+        <v>-4.3880967935570393E-25</v>
+      </c>
+      <c r="I10" s="9">
+        <f t="shared" si="0"/>
+        <v>-1.0268549830625926E-29</v>
+      </c>
+      <c r="J10" s="9">
+        <f t="shared" si="0"/>
+        <v>-4.3896548533046428E-25</v>
+      </c>
+      <c r="K10" s="9">
+        <f t="shared" si="0"/>
+        <v>-3.0254851388220243E-25</v>
+      </c>
+      <c r="L10" s="9">
+        <f t="shared" si="0"/>
+        <v>-4.9663922095752227E-28</v>
+      </c>
+      <c r="M10" s="9">
+        <f t="shared" si="0"/>
+        <v>-4.3896549762149814E-25</v>
+      </c>
+      <c r="N10" s="9">
+        <f t="shared" si="0"/>
+        <v>-4.3253252892730021E-25</v>
+      </c>
+      <c r="O10" s="9">
+        <f t="shared" si="0"/>
+        <v>-4.3896486902290552E-25</v>
+      </c>
+      <c r="P10" s="9">
+        <f t="shared" si="0"/>
+        <v>-8.778739385076152E-27</v>
+      </c>
+      <c r="Q10" s="9">
+        <f t="shared" si="0"/>
+        <v>-2.058027104001193E-31</v>
+      </c>
+      <c r="R10" s="9">
+        <f t="shared" si="0"/>
+        <v>-1.9252099850030676E-35</v>
+      </c>
+      <c r="S10" s="9">
+        <f t="shared" si="0"/>
+        <v>-4.3892595692636888E-25</v>
+      </c>
+      <c r="T10" s="9">
+        <f t="shared" si="0"/>
+        <v>-1.9529705713105641E-28</v>
+      </c>
+      <c r="U10" s="9">
+        <f t="shared" si="0"/>
+        <v>-4.3896548928115358E-25</v>
+      </c>
+      <c r="V10" s="9">
+        <f t="shared" si="0"/>
+        <v>-4.3391425228381881E-25</v>
+      </c>
+      <c r="W10" s="9">
+        <f t="shared" si="0"/>
+        <v>-4.3896549718253254E-25</v>
+      </c>
+      <c r="X10" s="9">
+        <f t="shared" si="0"/>
+        <v>-3.4899605851895427E-25</v>
+      </c>
+      <c r="Y10" s="9">
+        <f t="shared" si="0"/>
+        <v>-3.7270240338696822E-31</v>
+      </c>
+      <c r="Z10" s="9">
+        <f t="shared" si="0"/>
+        <v>-1.1072826585540265E-32</v>
+      </c>
+      <c r="AA10" s="9">
+        <f t="shared" ref="AA10:AF11" si="2">$B10*AA9</f>
+        <v>-4.3896549762149814E-25</v>
+      </c>
+      <c r="AB10" s="9">
+        <f t="shared" si="2"/>
+        <v>-4.1825541710921904E-25</v>
+      </c>
+      <c r="AC10" s="9">
+        <f t="shared" si="2"/>
+        <v>-4.3896463329843322E-25</v>
+      </c>
+      <c r="AD10" s="9">
+        <f t="shared" si="2"/>
+        <v>-9.1937403953894496E-29</v>
+      </c>
+      <c r="AE10" s="9">
+        <f t="shared" si="2"/>
+        <v>-1.3987665519155974E-29</v>
+      </c>
+      <c r="AF10" s="9">
+        <f t="shared" si="2"/>
+        <v>-9.4741620026489066E-35</v>
+      </c>
+    </row>
+    <row r="11" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>1.88102E-3</v>
+      </c>
+      <c r="C11" s="9">
+        <f t="shared" si="1"/>
+        <v>5.8049775244328001E-5</v>
+      </c>
+      <c r="D11" s="9">
+        <f t="shared" ref="D11:Z11" si="3">$B11*D10</f>
+        <v>-8.2570282171108581E-28</v>
+      </c>
+      <c r="E11" s="9">
+        <f t="shared" si="3"/>
+        <v>-2.4036666304289465E-28</v>
+      </c>
+      <c r="F11" s="9">
+        <f t="shared" si="3"/>
+        <v>-8.0897669635650061E-30</v>
+      </c>
+      <c r="G11" s="9">
+        <f t="shared" si="3"/>
+        <v>-8.195755712835265E-28</v>
+      </c>
+      <c r="H11" s="9">
+        <f t="shared" si="3"/>
+        <v>-8.2540978306166621E-28</v>
+      </c>
+      <c r="I11" s="9">
+        <f t="shared" si="3"/>
+        <v>-1.9315347602403978E-32</v>
+      </c>
+      <c r="J11" s="9">
+        <f t="shared" si="3"/>
+        <v>-8.2570285721630991E-28</v>
+      </c>
+      <c r="K11" s="9">
+        <f t="shared" si="3"/>
+        <v>-5.6909980558270035E-28</v>
+      </c>
+      <c r="L11" s="9">
+        <f t="shared" si="3"/>
+        <v>-9.341883074055185E-31</v>
+      </c>
+      <c r="M11" s="9">
+        <f t="shared" si="3"/>
+        <v>-8.2570288033599042E-28</v>
+      </c>
+      <c r="N11" s="9">
+        <f t="shared" si="3"/>
+        <v>-8.1360233756283016E-28</v>
+      </c>
+      <c r="O11" s="9">
+        <f t="shared" si="3"/>
+        <v>-8.2570169792946574E-28</v>
+      </c>
+      <c r="P11" s="9">
+        <f t="shared" si="3"/>
+        <v>-1.6512984358115942E-29</v>
+      </c>
+      <c r="Q11" s="9">
+        <f t="shared" si="3"/>
+        <v>-3.8711901431683237E-34</v>
+      </c>
+      <c r="R11" s="9">
+        <f t="shared" si="3"/>
+        <v>-3.6213584859904699E-38</v>
+      </c>
+      <c r="S11" s="9">
+        <f t="shared" si="3"/>
+        <v>-8.2562850349763843E-28</v>
+      </c>
+      <c r="T11" s="9">
+        <f t="shared" si="3"/>
+        <v>-3.6735767040465972E-31</v>
+      </c>
+      <c r="U11" s="9">
+        <f t="shared" si="3"/>
+        <v>-8.2570286464763539E-28</v>
+      </c>
+      <c r="V11" s="9">
+        <f t="shared" si="3"/>
+        <v>-8.1620138683090893E-28</v>
+      </c>
+      <c r="W11" s="9">
+        <f t="shared" si="3"/>
+        <v>-8.2570287951028743E-28</v>
+      </c>
+      <c r="X11" s="9">
+        <f t="shared" si="3"/>
+        <v>-6.5646856599532332E-28</v>
+      </c>
+      <c r="Y11" s="9">
+        <f t="shared" si="3"/>
+        <v>-7.0106067481895496E-34</v>
+      </c>
+      <c r="Z11" s="9">
+        <f t="shared" si="3"/>
+        <v>-2.0828208263932948E-35</v>
+      </c>
+      <c r="AA11" s="9">
+        <f t="shared" si="2"/>
+        <v>-8.2570288033599042E-28</v>
+      </c>
+      <c r="AB11" s="9">
+        <f t="shared" si="2"/>
+        <v>-7.8674680469078323E-28</v>
+      </c>
+      <c r="AC11" s="9">
+        <f t="shared" si="2"/>
+        <v>-8.2570125452701887E-28</v>
+      </c>
+      <c r="AD11" s="9">
+        <f t="shared" si="2"/>
+        <v>-1.7293609558535462E-31</v>
+      </c>
+      <c r="AE11" s="9">
+        <f t="shared" si="2"/>
+        <v>-2.6311078594842767E-32</v>
+      </c>
+      <c r="AF11" s="9">
+        <f t="shared" si="2"/>
+        <v>-1.7821088210222646E-37</v>
+      </c>
+    </row>
+    <row r="12" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="E12" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="13" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="14" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="E14" t="s">
+        <v>71</v>
+      </c>
+      <c r="F14" s="9"/>
+    </row>
+    <row r="15" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="E15" t="s">
+        <v>71</v>
+      </c>
+      <c r="F15" s="9"/>
+    </row>
+    <row r="16" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="E16" t="s">
+        <v>71</v>
+      </c>
+      <c r="F16" s="9"/>
+    </row>
+    <row r="17" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E17" t="s">
+        <v>71</v>
+      </c>
+      <c r="F17" s="9"/>
+    </row>
+    <row r="18" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E18" t="s">
+        <v>71</v>
+      </c>
+      <c r="F18" s="9"/>
+    </row>
+    <row r="19" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E19" t="s">
+        <v>71</v>
+      </c>
+      <c r="F19" s="9"/>
+    </row>
+    <row r="20" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E20" t="s">
+        <v>71</v>
+      </c>
+      <c r="F20" s="9"/>
+    </row>
+    <row r="21" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E21" t="s">
+        <v>71</v>
+      </c>
+      <c r="F21" s="9"/>
+    </row>
+    <row r="22" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E22" t="s">
+        <v>71</v>
+      </c>
+      <c r="F22" s="9"/>
+    </row>
+    <row r="23" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E23" t="s">
+        <v>71</v>
+      </c>
+      <c r="F23" s="9"/>
+    </row>
+    <row r="24" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E24" t="s">
+        <v>71</v>
+      </c>
+      <c r="F24" s="9"/>
+    </row>
+    <row r="25" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E25" t="s">
+        <v>71</v>
+      </c>
+      <c r="F25" s="9"/>
+    </row>
+    <row r="26" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E26" t="s">
+        <v>71</v>
+      </c>
+      <c r="F26" s="9"/>
+    </row>
+    <row r="27" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E27" t="s">
+        <v>71</v>
+      </c>
+      <c r="F27" s="9"/>
+    </row>
+    <row r="28" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E28" t="s">
+        <v>71</v>
+      </c>
+      <c r="F28" s="9"/>
+    </row>
+    <row r="29" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E29" t="s">
+        <v>71</v>
+      </c>
+      <c r="F29" s="9"/>
+    </row>
+    <row r="30" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E30" t="s">
+        <v>71</v>
+      </c>
+      <c r="F30" s="9"/>
+    </row>
+    <row r="31" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="F31" s="9"/>
+    </row>
+    <row r="32" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="F32" s="9"/>
+    </row>
+    <row r="33" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F33" s="9"/>
+    </row>
+    <row r="34" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F34" s="9"/>
+    </row>
+    <row r="35" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F35" s="9"/>
+    </row>
+    <row r="36" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F36" s="9"/>
+    </row>
+    <row r="37" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F37" s="9"/>
+    </row>
+    <row r="38" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F38" s="9"/>
+    </row>
+    <row r="39" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F39" s="9"/>
+    </row>
+    <row r="40" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F40" s="9"/>
+    </row>
+    <row r="41" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F41" s="9"/>
+    </row>
+    <row r="42" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F42" s="9"/>
+    </row>
+    <row r="43" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F43" s="9"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C7E19DF-6C07-4938-AC54-C7F41D25C312}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2016,12 +3561,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G21"/>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2089,48 +3634,48 @@
       <c r="B8">
         <v>1</v>
       </c>
-      <c r="C8">
-        <v>0.51721518182005644</v>
+      <c r="C8" s="6">
+        <v>0.5</v>
       </c>
       <c r="D8" s="3">
         <f>L0*C8</f>
-        <v>2.0688607272802257</v>
+        <v>2</v>
       </c>
       <c r="E8" s="3">
         <f>1/(1+EXP(-D8))</f>
-        <v>0.88783956224387894</v>
+        <v>0.88079707797788231</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>2</v>
       </c>
-      <c r="C9">
-        <v>0.50109152103123156</v>
+      <c r="C9" s="6">
+        <v>0.5</v>
       </c>
       <c r="D9" s="3">
         <f>E8*C9</f>
-        <v>0.44488887667648808</v>
+        <v>0.44039853898894116</v>
       </c>
       <c r="E9" s="3">
         <f>1/(1+EXP(-D9))</f>
-        <v>0.60942333365042256</v>
+        <v>0.60835399051139183</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>3</v>
       </c>
-      <c r="C10">
-        <v>0.51720999828656755</v>
+      <c r="C10" s="6">
+        <v>0.5</v>
       </c>
       <c r="D10" s="3">
         <f>E9*C10</f>
-        <v>0.31519984135312934</v>
+        <v>0.30417699525569591</v>
       </c>
       <c r="E10" s="3">
         <f>1/(1+EXP(-D10))</f>
-        <v>0.5781539733439891</v>
+        <v>0.57546329912743177</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -2156,19 +3701,19 @@
       </c>
       <c r="C13">
         <f>(E10-$C$2)*(1/(1+EXP(-E10))*(1-(1/(1+EXP(-E10)))))</f>
-        <v>-1.4784353381213871</v>
+        <v>-1.4801721576676283</v>
       </c>
       <c r="D13">
         <f>C13*C9</f>
-        <v>-0.74083141232556893</v>
+        <v>-0.74008607883381416</v>
       </c>
       <c r="E13">
         <f>C13*E10</f>
-        <v>-0.85476326506704392</v>
+        <v>-0.85178475312798252</v>
       </c>
       <c r="F13">
         <f>C10-$C$3*E13</f>
-        <v>0.52575763093723804</v>
+        <v>0.50851784753127982</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -2177,19 +3722,19 @@
       </c>
       <c r="C14">
         <f>(C13*C10)*(1/(1+EXP(-D9))*(1-(1/(1+EXP(-D9)))))</f>
-        <v>-0.18200973577944565</v>
+        <v>-0.17633247452018427</v>
       </c>
       <c r="D14">
         <f>C14*E8</f>
-        <v>-0.1615954441385471</v>
+        <v>-0.1553131283099877</v>
       </c>
       <c r="E14">
         <f>C14*E9</f>
-        <v>-0.11092097993554235</v>
+        <v>-0.10727256453110243</v>
       </c>
       <c r="F14">
         <f>C19-$C$3*E14</f>
-        <v>0.50110920979935547</v>
+        <v>0.50107272564531102</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -2198,19 +3743,19 @@
       </c>
       <c r="C15">
         <f>(C14*C9)*(1/(1+EXP(-D8))*(1-(1/(1+EXP(-D8)))))</f>
-        <v>-9.0820912762655786E-3</v>
+        <v>-9.2568893614733104E-3</v>
       </c>
       <c r="D15">
         <f>C15*L0</f>
-        <v>-3.6328365105062314E-2</v>
+        <v>-3.7027557445893242E-2</v>
       </c>
       <c r="E15">
         <f>C15*E8</f>
-        <v>-8.0634399429785827E-3</v>
+        <v>-8.1534411007502371E-3</v>
       </c>
       <c r="F15">
         <f>C8-$C$3*E15</f>
-        <v>0.51729581621948617</v>
+        <v>0.50008153441100756</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -2218,7 +3763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
         <v>67</v>
       </c>
@@ -2232,55 +3777,19 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C19" s="6">
         <v>0.5</v>
       </c>
-      <c r="D19">
-        <v>0.50851784753127982</v>
-      </c>
-      <c r="E19">
-        <v>0.50860039221460152</v>
-      </c>
-      <c r="F19">
-        <v>0.51713063151095084</v>
-      </c>
-      <c r="G19">
-        <v>0.51721518182005644</v>
-      </c>
-    </row>
-    <row r="20" spans="3:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C20" s="6">
         <v>0.5</v>
       </c>
-      <c r="D20">
-        <v>0.50107272564531102</v>
-      </c>
-      <c r="E20">
-        <v>0.50107336469369013</v>
-      </c>
-      <c r="F20">
-        <v>0.50109104405172933</v>
-      </c>
-      <c r="G20">
-        <v>0.50109152103123156</v>
-      </c>
-    </row>
-    <row r="21" spans="3:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C21" s="6">
         <v>0.5</v>
-      </c>
-      <c r="D21">
-        <v>0.50008153441100756</v>
-      </c>
-      <c r="E21">
-        <v>0.50859773614299053</v>
-      </c>
-      <c r="F21">
-        <v>0.50868157871043673</v>
-      </c>
-      <c r="G21">
-        <v>0.51720999828656755</v>
       </c>
     </row>
   </sheetData>

</xml_diff>